<commit_message>
20191118 - Gravity Attempt #1 (in progress)
</commit_message>
<xml_diff>
--- a/res/references/First Platformer Checklist.xlsx
+++ b/res/references/First Platformer Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apauley\git\platforming101\res\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8CDAD0-8C5C-4D88-8CDD-1CF5CC34AC68}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3C5342-066A-42BC-AE1F-A1F56F8F5B4F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2565" windowWidth="28695" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -1212,45 +1212,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1302,6 +1263,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1711,7 +1711,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1735,19 +1735,19 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="147" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="127"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="149"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="158" t="s">
+      <c r="B3" s="125"/>
+      <c r="C3" s="145" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="123"/>
@@ -1758,14 +1758,14 @@
     <row r="4" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="138"/>
-      <c r="D4" s="140">
+      <c r="C4" s="125"/>
+      <c r="D4" s="127">
         <v>0</v>
       </c>
-      <c r="E4" s="139" t="s">
+      <c r="E4" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="141" t="s">
+      <c r="F4" s="128" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="4"/>
@@ -1773,14 +1773,14 @@
     <row r="5" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="138"/>
-      <c r="D5" s="142">
+      <c r="C5" s="125"/>
+      <c r="D5" s="129">
         <v>1</v>
       </c>
-      <c r="E5" s="143" t="s">
+      <c r="E5" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="144" t="s">
+      <c r="F5" s="131" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="4"/>
@@ -1788,14 +1788,14 @@
     <row r="6" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="138"/>
-      <c r="D6" s="140">
+      <c r="C6" s="125"/>
+      <c r="D6" s="127">
         <v>2</v>
       </c>
-      <c r="E6" s="139" t="s">
+      <c r="E6" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="141" t="s">
+      <c r="F6" s="128" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="4"/>
@@ -1803,14 +1803,14 @@
     <row r="7" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="142">
+      <c r="C7" s="125"/>
+      <c r="D7" s="129">
         <v>3</v>
       </c>
-      <c r="E7" s="143" t="s">
+      <c r="E7" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="144" t="s">
+      <c r="F7" s="131" t="s">
         <v>62</v>
       </c>
       <c r="G7" s="4"/>
@@ -1818,14 +1818,14 @@
     <row r="8" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="145">
+      <c r="C8" s="125"/>
+      <c r="D8" s="132">
         <v>4</v>
       </c>
-      <c r="E8" s="146" t="s">
+      <c r="E8" s="133" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="147" t="s">
+      <c r="F8" s="134" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="4"/>
@@ -1834,33 +1834,33 @@
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="148"/>
-      <c r="E9" s="148"/>
-      <c r="F9" s="149"/>
+      <c r="D9" s="135"/>
+      <c r="E9" s="135"/>
+      <c r="F9" s="136"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="7"/>
-      <c r="C10" s="157" t="s">
+      <c r="C10" s="144" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="150"/>
-      <c r="E10" s="150"/>
-      <c r="F10" s="151"/>
+      <c r="D10" s="137"/>
+      <c r="E10" s="137"/>
+      <c r="F10" s="138"/>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="140">
+      <c r="C11" s="125"/>
+      <c r="D11" s="127">
         <v>5</v>
       </c>
-      <c r="E11" s="139" t="s">
+      <c r="E11" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="141" t="s">
+      <c r="F11" s="128" t="s">
         <v>4</v>
       </c>
       <c r="G11" s="4"/>
@@ -1869,13 +1869,13 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="142">
+      <c r="D12" s="129">
         <v>6</v>
       </c>
-      <c r="E12" s="143" t="s">
+      <c r="E12" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="144" t="s">
+      <c r="F12" s="131" t="s">
         <v>5</v>
       </c>
       <c r="G12" s="4"/>
@@ -1884,13 +1884,13 @@
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="140">
+      <c r="D13" s="127">
         <v>7</v>
       </c>
-      <c r="E13" s="139" t="s">
+      <c r="E13" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="141" t="s">
+      <c r="F13" s="128" t="s">
         <v>6</v>
       </c>
       <c r="G13" s="4"/>
@@ -1899,13 +1899,13 @@
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="152">
+      <c r="D14" s="139">
         <v>8</v>
       </c>
-      <c r="E14" s="153" t="s">
+      <c r="E14" s="140" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="154" t="s">
+      <c r="F14" s="141" t="s">
         <v>9</v>
       </c>
       <c r="G14" s="4"/>
@@ -1914,33 +1914,33 @@
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="148"/>
-      <c r="E15" s="148"/>
-      <c r="F15" s="149"/>
+      <c r="D15" s="135"/>
+      <c r="E15" s="135"/>
+      <c r="F15" s="136"/>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="158" t="s">
+      <c r="C16" s="145" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="155"/>
-      <c r="E16" s="155"/>
-      <c r="F16" s="156"/>
+      <c r="D16" s="142"/>
+      <c r="E16" s="142"/>
+      <c r="F16" s="143"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="140">
+      <c r="D17" s="127">
         <v>9</v>
       </c>
-      <c r="E17" s="139" t="s">
+      <c r="E17" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="141" t="s">
+      <c r="F17" s="128" t="s">
         <v>11</v>
       </c>
       <c r="G17" s="4"/>
@@ -1949,13 +1949,13 @@
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="142">
+      <c r="D18" s="129">
         <v>10</v>
       </c>
-      <c r="E18" s="143" t="s">
+      <c r="E18" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="144" t="s">
+      <c r="F18" s="131" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="4"/>
@@ -1964,13 +1964,13 @@
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
-      <c r="D19" s="140">
+      <c r="D19" s="127">
         <v>11</v>
       </c>
-      <c r="E19" s="139" t="s">
+      <c r="E19" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="141" t="s">
+      <c r="F19" s="128" t="s">
         <v>12</v>
       </c>
       <c r="G19" s="4"/>
@@ -1979,13 +1979,13 @@
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="142">
+      <c r="D20" s="129">
         <v>12</v>
       </c>
-      <c r="E20" s="143" t="s">
+      <c r="E20" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="144" t="s">
+      <c r="F20" s="131" t="s">
         <v>15</v>
       </c>
       <c r="G20" s="4"/>
@@ -1994,13 +1994,13 @@
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="140">
+      <c r="D21" s="127">
         <v>13</v>
       </c>
-      <c r="E21" s="139" t="s">
+      <c r="E21" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F21" s="141" t="s">
+      <c r="F21" s="128" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="4"/>
@@ -2009,13 +2009,13 @@
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
-      <c r="D22" s="145">
+      <c r="D22" s="132">
         <v>14</v>
       </c>
-      <c r="E22" s="146" t="s">
+      <c r="E22" s="133" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="147" t="s">
+      <c r="F22" s="134" t="s">
         <v>17</v>
       </c>
       <c r="G22" s="4"/>
@@ -2024,33 +2024,33 @@
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="148"/>
-      <c r="E23" s="148"/>
-      <c r="F23" s="149"/>
+      <c r="D23" s="135"/>
+      <c r="E23" s="135"/>
+      <c r="F23" s="136"/>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="7"/>
-      <c r="C24" s="157" t="s">
+      <c r="C24" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="150"/>
-      <c r="E24" s="150"/>
-      <c r="F24" s="151"/>
+      <c r="D24" s="137"/>
+      <c r="E24" s="137"/>
+      <c r="F24" s="138"/>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="9"/>
-      <c r="D25" s="140">
+      <c r="D25" s="127">
         <v>15</v>
       </c>
-      <c r="E25" s="139" t="s">
+      <c r="E25" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="141" t="s">
+      <c r="F25" s="128" t="s">
         <v>19</v>
       </c>
       <c r="G25" s="4"/>
@@ -2059,13 +2059,13 @@
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="8"/>
-      <c r="D26" s="142">
+      <c r="D26" s="129">
         <v>16</v>
       </c>
-      <c r="E26" s="143" t="s">
+      <c r="E26" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="144" t="s">
+      <c r="F26" s="131" t="s">
         <v>20</v>
       </c>
       <c r="G26" s="4"/>
@@ -2074,13 +2074,13 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="140">
+      <c r="D27" s="127">
         <v>17</v>
       </c>
-      <c r="E27" s="139" t="s">
+      <c r="E27" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="141" t="s">
+      <c r="F27" s="128" t="s">
         <v>21</v>
       </c>
       <c r="G27" s="4"/>
@@ -2089,13 +2089,13 @@
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="142">
+      <c r="D28" s="129">
         <v>18</v>
       </c>
-      <c r="E28" s="143" t="s">
+      <c r="E28" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="144" t="s">
+      <c r="F28" s="131" t="s">
         <v>22</v>
       </c>
       <c r="G28" s="4"/>
@@ -2104,13 +2104,13 @@
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="140">
+      <c r="D29" s="127">
         <v>19</v>
       </c>
-      <c r="E29" s="139" t="s">
+      <c r="E29" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="141" t="s">
+      <c r="F29" s="128" t="s">
         <v>23</v>
       </c>
       <c r="G29" s="4"/>
@@ -2119,13 +2119,13 @@
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="142">
+      <c r="D30" s="129">
         <v>20</v>
       </c>
-      <c r="E30" s="143" t="s">
+      <c r="E30" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="144" t="s">
+      <c r="F30" s="131" t="s">
         <v>24</v>
       </c>
       <c r="G30" s="4"/>
@@ -2134,13 +2134,13 @@
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="8"/>
-      <c r="D31" s="140">
+      <c r="D31" s="127">
         <v>21</v>
       </c>
-      <c r="E31" s="139" t="s">
+      <c r="E31" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="141" t="s">
+      <c r="F31" s="128" t="s">
         <v>25</v>
       </c>
       <c r="G31" s="4"/>
@@ -2149,13 +2149,13 @@
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="8"/>
-      <c r="D32" s="140">
+      <c r="D32" s="127">
         <v>22</v>
       </c>
-      <c r="E32" s="139" t="s">
+      <c r="E32" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="141" t="s">
+      <c r="F32" s="128" t="s">
         <v>26</v>
       </c>
       <c r="G32" s="4"/>
@@ -2164,13 +2164,13 @@
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="152">
+      <c r="D33" s="139">
         <v>23</v>
       </c>
-      <c r="E33" s="153" t="s">
+      <c r="E33" s="140" t="s">
         <v>35</v>
       </c>
-      <c r="F33" s="154" t="s">
+      <c r="F33" s="141" t="s">
         <v>48</v>
       </c>
       <c r="G33" s="4"/>
@@ -2178,34 +2178,34 @@
     <row r="34" spans="1:7" ht="3.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
-      <c r="C34" s="159"/>
-      <c r="D34" s="148"/>
-      <c r="E34" s="148"/>
-      <c r="F34" s="149"/>
+      <c r="C34" s="146"/>
+      <c r="D34" s="135"/>
+      <c r="E34" s="135"/>
+      <c r="F34" s="136"/>
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="7"/>
-      <c r="C35" s="158" t="s">
+      <c r="C35" s="145" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="155"/>
-      <c r="E35" s="155"/>
-      <c r="F35" s="156"/>
+      <c r="D35" s="142"/>
+      <c r="E35" s="142"/>
+      <c r="F35" s="143"/>
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="9"/>
-      <c r="D36" s="140">
+      <c r="D36" s="127">
         <v>24</v>
       </c>
-      <c r="E36" s="139" t="s">
+      <c r="E36" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F36" s="141" t="s">
+      <c r="F36" s="128" t="s">
         <v>28</v>
       </c>
       <c r="G36" s="4"/>
@@ -2214,13 +2214,13 @@
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="142">
+      <c r="D37" s="129">
         <v>25</v>
       </c>
-      <c r="E37" s="143" t="s">
+      <c r="E37" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F37" s="144" t="s">
+      <c r="F37" s="131" t="s">
         <v>29</v>
       </c>
       <c r="G37" s="4"/>
@@ -2229,13 +2229,13 @@
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="8"/>
-      <c r="D38" s="140">
+      <c r="D38" s="127">
         <v>26</v>
       </c>
-      <c r="E38" s="139" t="s">
+      <c r="E38" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F38" s="141" t="s">
+      <c r="F38" s="128" t="s">
         <v>30</v>
       </c>
       <c r="G38" s="4"/>
@@ -2244,13 +2244,13 @@
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="142">
+      <c r="D39" s="129">
         <v>27</v>
       </c>
-      <c r="E39" s="143" t="s">
+      <c r="E39" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F39" s="144" t="s">
+      <c r="F39" s="131" t="s">
         <v>31</v>
       </c>
       <c r="G39" s="4"/>
@@ -2259,13 +2259,13 @@
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="8"/>
-      <c r="D40" s="140">
+      <c r="D40" s="127">
         <v>28</v>
       </c>
-      <c r="E40" s="139" t="s">
+      <c r="E40" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F40" s="141" t="s">
+      <c r="F40" s="128" t="s">
         <v>32</v>
       </c>
       <c r="G40" s="4"/>
@@ -2274,13 +2274,13 @@
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="8"/>
-      <c r="D41" s="142">
+      <c r="D41" s="129">
         <v>29</v>
       </c>
-      <c r="E41" s="143" t="s">
+      <c r="E41" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F41" s="144" t="s">
+      <c r="F41" s="131" t="s">
         <v>33</v>
       </c>
       <c r="G41" s="4"/>
@@ -2289,13 +2289,13 @@
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="140">
+      <c r="D42" s="127">
         <v>30</v>
       </c>
-      <c r="E42" s="139" t="s">
+      <c r="E42" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F42" s="141" t="s">
+      <c r="F42" s="128" t="s">
         <v>63</v>
       </c>
       <c r="G42" s="4"/>
@@ -2304,13 +2304,13 @@
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="8"/>
-      <c r="D43" s="152">
+      <c r="D43" s="139">
         <v>31</v>
       </c>
-      <c r="E43" s="153" t="s">
+      <c r="E43" s="140" t="s">
         <v>35</v>
       </c>
-      <c r="F43" s="154" t="s">
+      <c r="F43" s="141" t="s">
         <v>34</v>
       </c>
       <c r="G43" s="4"/>
@@ -2380,7 +2380,9 @@
   </sheetPr>
   <dimension ref="B2:P50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="W53" sqref="W53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2985,8 +2987,8 @@
   </sheetPr>
   <dimension ref="B2:O40"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4744,12 +4746,12 @@
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="70"/>
       <c r="C45" s="77"/>
-      <c r="D45" s="128" t="s">
+      <c r="D45" s="150" t="s">
         <v>41</v>
       </c>
-      <c r="E45" s="128"/>
-      <c r="F45" s="128"/>
-      <c r="G45" s="128"/>
+      <c r="E45" s="150"/>
+      <c r="F45" s="150"/>
+      <c r="G45" s="150"/>
       <c r="H45" s="77"/>
       <c r="I45" s="56"/>
       <c r="O45" s="12"/>
@@ -4757,12 +4759,12 @@
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="70"/>
       <c r="C46" s="77"/>
-      <c r="D46" s="129" t="s">
+      <c r="D46" s="151" t="s">
         <v>42</v>
       </c>
-      <c r="E46" s="130"/>
-      <c r="F46" s="130"/>
-      <c r="G46" s="130"/>
+      <c r="E46" s="152"/>
+      <c r="F46" s="152"/>
+      <c r="G46" s="152"/>
       <c r="H46" s="77"/>
       <c r="I46" s="56"/>
       <c r="O46" s="12"/>
@@ -4770,12 +4772,12 @@
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="70"/>
       <c r="C47" s="77"/>
-      <c r="D47" s="132" t="s">
+      <c r="D47" s="154" t="s">
         <v>44</v>
       </c>
-      <c r="E47" s="132"/>
-      <c r="F47" s="132"/>
-      <c r="G47" s="132"/>
+      <c r="E47" s="154"/>
+      <c r="F47" s="154"/>
+      <c r="G47" s="154"/>
       <c r="H47" s="77"/>
       <c r="I47" s="56"/>
       <c r="N47" s="61"/>
@@ -4784,12 +4786,12 @@
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="70"/>
       <c r="C48" s="77"/>
-      <c r="D48" s="129" t="s">
+      <c r="D48" s="151" t="s">
         <v>43</v>
       </c>
-      <c r="E48" s="129"/>
-      <c r="F48" s="129"/>
-      <c r="G48" s="129"/>
+      <c r="E48" s="151"/>
+      <c r="F48" s="151"/>
+      <c r="G48" s="151"/>
       <c r="H48" s="77"/>
       <c r="I48" s="75"/>
       <c r="J48" s="12"/>
@@ -4992,26 +4994,26 @@
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B65" s="70"/>
-      <c r="C65" s="131" t="s">
+      <c r="C65" s="153" t="s">
         <v>47</v>
       </c>
-      <c r="D65" s="131"/>
-      <c r="E65" s="131"/>
-      <c r="F65" s="131"/>
-      <c r="G65" s="131"/>
-      <c r="H65" s="131"/>
+      <c r="D65" s="153"/>
+      <c r="E65" s="153"/>
+      <c r="F65" s="153"/>
+      <c r="G65" s="153"/>
+      <c r="H65" s="153"/>
       <c r="I65" s="56"/>
       <c r="O65" s="12"/>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="70"/>
       <c r="C66" s="77"/>
-      <c r="D66" s="128" t="s">
+      <c r="D66" s="150" t="s">
         <v>45</v>
       </c>
-      <c r="E66" s="128"/>
-      <c r="F66" s="128"/>
-      <c r="G66" s="128"/>
+      <c r="E66" s="150"/>
+      <c r="F66" s="150"/>
+      <c r="G66" s="150"/>
       <c r="H66" s="77"/>
       <c r="I66" s="56"/>
       <c r="O66" s="12"/>
@@ -5019,12 +5021,12 @@
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B67" s="70"/>
       <c r="C67" s="77"/>
-      <c r="D67" s="129" t="s">
+      <c r="D67" s="151" t="s">
         <v>46</v>
       </c>
-      <c r="E67" s="130"/>
-      <c r="F67" s="130"/>
-      <c r="G67" s="130"/>
+      <c r="E67" s="152"/>
+      <c r="F67" s="152"/>
+      <c r="G67" s="152"/>
       <c r="H67" s="77"/>
       <c r="I67" s="56"/>
       <c r="N67" s="29"/>
@@ -5033,12 +5035,12 @@
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B68" s="70"/>
       <c r="C68" s="77"/>
-      <c r="D68" s="129" t="s">
+      <c r="D68" s="151" t="s">
         <v>43</v>
       </c>
-      <c r="E68" s="129"/>
-      <c r="F68" s="129"/>
-      <c r="G68" s="129"/>
+      <c r="E68" s="151"/>
+      <c r="F68" s="151"/>
+      <c r="G68" s="151"/>
       <c r="H68" s="77"/>
       <c r="I68" s="56"/>
       <c r="J68" s="12"/>
@@ -6110,77 +6112,77 @@
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="33"/>
       <c r="C44" s="77"/>
-      <c r="D44" s="133" t="s">
+      <c r="D44" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="133"/>
-      <c r="F44" s="133"/>
-      <c r="G44" s="133"/>
+      <c r="E44" s="159"/>
+      <c r="F44" s="159"/>
+      <c r="G44" s="159"/>
       <c r="H44" s="77"/>
       <c r="I44" s="35"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="33"/>
-      <c r="C45" s="134" t="s">
+      <c r="C45" s="157" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="134"/>
+      <c r="D45" s="157"/>
       <c r="E45" s="121" t="s">
         <v>54</v>
       </c>
-      <c r="F45" s="134">
+      <c r="F45" s="157">
         <v>9001</v>
       </c>
-      <c r="G45" s="134"/>
-      <c r="H45" s="134"/>
+      <c r="G45" s="157"/>
+      <c r="H45" s="157"/>
       <c r="I45" s="35"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="33"/>
-      <c r="C46" s="135" t="s">
+      <c r="C46" s="155" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="135"/>
+      <c r="D46" s="155"/>
       <c r="E46" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="F46" s="135">
+      <c r="F46" s="155">
         <v>8999</v>
       </c>
-      <c r="G46" s="135"/>
-      <c r="H46" s="135"/>
+      <c r="G46" s="155"/>
+      <c r="H46" s="155"/>
       <c r="I46" s="35"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="33"/>
-      <c r="C47" s="135" t="s">
+      <c r="C47" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="135"/>
+      <c r="D47" s="155"/>
       <c r="E47" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="F47" s="135">
+      <c r="F47" s="155">
         <v>1337</v>
       </c>
-      <c r="G47" s="135"/>
-      <c r="H47" s="135"/>
+      <c r="G47" s="155"/>
+      <c r="H47" s="155"/>
       <c r="I47" s="35"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="33"/>
-      <c r="C48" s="135" t="s">
+      <c r="C48" s="155" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="135"/>
+      <c r="D48" s="155"/>
       <c r="E48" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="F48" s="135">
+      <c r="F48" s="155">
         <v>-5</v>
       </c>
-      <c r="G48" s="135"/>
-      <c r="H48" s="135"/>
+      <c r="G48" s="155"/>
+      <c r="H48" s="155"/>
       <c r="I48" s="35"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
@@ -6249,12 +6251,12 @@
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="90"/>
       <c r="C55" s="77"/>
-      <c r="D55" s="128" t="s">
+      <c r="D55" s="150" t="s">
         <v>41</v>
       </c>
-      <c r="E55" s="128"/>
-      <c r="F55" s="128"/>
-      <c r="G55" s="128"/>
+      <c r="E55" s="150"/>
+      <c r="F55" s="150"/>
+      <c r="G55" s="150"/>
       <c r="H55" s="77"/>
       <c r="I55" s="82"/>
       <c r="J55" s="83"/>
@@ -6267,12 +6269,12 @@
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" s="90"/>
       <c r="C56" s="77"/>
-      <c r="D56" s="129" t="s">
+      <c r="D56" s="151" t="s">
         <v>42</v>
       </c>
-      <c r="E56" s="130"/>
-      <c r="F56" s="130"/>
-      <c r="G56" s="130"/>
+      <c r="E56" s="152"/>
+      <c r="F56" s="152"/>
+      <c r="G56" s="152"/>
       <c r="H56" s="77"/>
       <c r="I56" s="82"/>
       <c r="J56" s="83"/>
@@ -6285,12 +6287,12 @@
     <row r="57" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="90"/>
       <c r="C57" s="77"/>
-      <c r="D57" s="129" t="s">
+      <c r="D57" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="E57" s="130"/>
-      <c r="F57" s="130"/>
-      <c r="G57" s="130"/>
+      <c r="E57" s="152"/>
+      <c r="F57" s="152"/>
+      <c r="G57" s="152"/>
       <c r="H57" s="77"/>
       <c r="I57" s="82"/>
       <c r="J57" s="83"/>
@@ -6303,12 +6305,12 @@
     <row r="58" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="90"/>
       <c r="C58" s="77"/>
-      <c r="D58" s="132" t="s">
+      <c r="D58" s="154" t="s">
         <v>60</v>
       </c>
-      <c r="E58" s="132"/>
-      <c r="F58" s="132"/>
-      <c r="G58" s="132"/>
+      <c r="E58" s="154"/>
+      <c r="F58" s="154"/>
+      <c r="G58" s="154"/>
       <c r="H58" s="77"/>
       <c r="I58" s="89"/>
       <c r="J58" s="87"/>
@@ -6377,14 +6379,14 @@
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B64" s="33"/>
-      <c r="C64" s="128" t="s">
+      <c r="C64" s="150" t="s">
         <v>64</v>
       </c>
-      <c r="D64" s="128"/>
-      <c r="E64" s="128"/>
-      <c r="F64" s="128"/>
-      <c r="G64" s="128"/>
-      <c r="H64" s="128"/>
+      <c r="D64" s="150"/>
+      <c r="E64" s="150"/>
+      <c r="F64" s="150"/>
+      <c r="G64" s="150"/>
+      <c r="H64" s="150"/>
       <c r="I64" s="35"/>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
@@ -6399,50 +6401,50 @@
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="33"/>
-      <c r="C66" s="135" t="s">
+      <c r="C66" s="155" t="s">
         <v>65</v>
       </c>
-      <c r="D66" s="135"/>
+      <c r="D66" s="155"/>
       <c r="E66" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="F66" s="136" t="s">
+      <c r="F66" s="156" t="s">
         <v>66</v>
       </c>
-      <c r="G66" s="136"/>
-      <c r="H66" s="136"/>
+      <c r="G66" s="156"/>
+      <c r="H66" s="156"/>
       <c r="I66" s="35"/>
     </row>
     <row r="67" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="33"/>
-      <c r="C67" s="134" t="s">
+      <c r="C67" s="157" t="s">
         <v>68</v>
       </c>
-      <c r="D67" s="134"/>
+      <c r="D67" s="157"/>
       <c r="E67" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="F67" s="137" t="s">
+      <c r="F67" s="158" t="s">
         <v>66</v>
       </c>
-      <c r="G67" s="137"/>
-      <c r="H67" s="137"/>
+      <c r="G67" s="158"/>
+      <c r="H67" s="158"/>
       <c r="I67" s="35"/>
     </row>
     <row r="68" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="33"/>
-      <c r="C68" s="135" t="s">
+      <c r="C68" s="155" t="s">
         <v>67</v>
       </c>
-      <c r="D68" s="135"/>
+      <c r="D68" s="155"/>
       <c r="E68" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="F68" s="136" t="s">
+      <c r="F68" s="156" t="s">
         <v>66</v>
       </c>
-      <c r="G68" s="136"/>
-      <c r="H68" s="136"/>
+      <c r="G68" s="156"/>
+      <c r="H68" s="156"/>
       <c r="I68" s="35"/>
     </row>
     <row r="69" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7278,13 +7280,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="C64:H64"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="F67:H67"/>
     <mergeCell ref="D44:G44"/>
     <mergeCell ref="D57:G57"/>
     <mergeCell ref="D58:G58"/>
@@ -7298,6 +7293,13 @@
     <mergeCell ref="F47:H47"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="F48:H48"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="C64:H64"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="F67:H67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
20191119 - Added Creature/Player Facing
As well as related debug visuals and text
</commit_message>
<xml_diff>
--- a/res/references/First Platformer Checklist.xlsx
+++ b/res/references/First Platformer Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apauley\git\platforming101\res\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3C5342-066A-42BC-AE1F-A1F56F8F5B4F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D097E5-6092-455E-9C03-12C37899D8D0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2565" windowWidth="28695" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="105" yWindow="1935" windowWidth="28695" windowHeight="11745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -1288,19 +1288,19 @@
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1711,7 +1711,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1868,7 +1868,7 @@
     <row r="12" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="8"/>
+      <c r="C12" s="125"/>
       <c r="D12" s="129">
         <v>6</v>
       </c>
@@ -1898,7 +1898,7 @@
     <row r="14" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="8"/>
+      <c r="C14" s="125"/>
       <c r="D14" s="139">
         <v>8</v>
       </c>
@@ -6112,77 +6112,77 @@
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="33"/>
       <c r="C44" s="77"/>
-      <c r="D44" s="159" t="s">
+      <c r="D44" s="155" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="159"/>
-      <c r="F44" s="159"/>
-      <c r="G44" s="159"/>
+      <c r="E44" s="155"/>
+      <c r="F44" s="155"/>
+      <c r="G44" s="155"/>
       <c r="H44" s="77"/>
       <c r="I44" s="35"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="33"/>
-      <c r="C45" s="157" t="s">
+      <c r="C45" s="156" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="157"/>
+      <c r="D45" s="156"/>
       <c r="E45" s="121" t="s">
         <v>54</v>
       </c>
-      <c r="F45" s="157">
+      <c r="F45" s="156">
         <v>9001</v>
       </c>
-      <c r="G45" s="157"/>
-      <c r="H45" s="157"/>
+      <c r="G45" s="156"/>
+      <c r="H45" s="156"/>
       <c r="I45" s="35"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="33"/>
-      <c r="C46" s="155" t="s">
+      <c r="C46" s="157" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="155"/>
+      <c r="D46" s="157"/>
       <c r="E46" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="F46" s="155">
+      <c r="F46" s="157">
         <v>8999</v>
       </c>
-      <c r="G46" s="155"/>
-      <c r="H46" s="155"/>
+      <c r="G46" s="157"/>
+      <c r="H46" s="157"/>
       <c r="I46" s="35"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="33"/>
-      <c r="C47" s="155" t="s">
+      <c r="C47" s="157" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="155"/>
+      <c r="D47" s="157"/>
       <c r="E47" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="F47" s="155">
+      <c r="F47" s="157">
         <v>1337</v>
       </c>
-      <c r="G47" s="155"/>
-      <c r="H47" s="155"/>
+      <c r="G47" s="157"/>
+      <c r="H47" s="157"/>
       <c r="I47" s="35"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="33"/>
-      <c r="C48" s="155" t="s">
+      <c r="C48" s="157" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="155"/>
+      <c r="D48" s="157"/>
       <c r="E48" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="F48" s="155">
+      <c r="F48" s="157">
         <v>-5</v>
       </c>
-      <c r="G48" s="155"/>
-      <c r="H48" s="155"/>
+      <c r="G48" s="157"/>
+      <c r="H48" s="157"/>
       <c r="I48" s="35"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
@@ -6401,50 +6401,50 @@
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="33"/>
-      <c r="C66" s="155" t="s">
+      <c r="C66" s="157" t="s">
         <v>65</v>
       </c>
-      <c r="D66" s="155"/>
+      <c r="D66" s="157"/>
       <c r="E66" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="F66" s="156" t="s">
+      <c r="F66" s="158" t="s">
         <v>66</v>
       </c>
-      <c r="G66" s="156"/>
-      <c r="H66" s="156"/>
+      <c r="G66" s="158"/>
+      <c r="H66" s="158"/>
       <c r="I66" s="35"/>
     </row>
     <row r="67" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="33"/>
-      <c r="C67" s="157" t="s">
+      <c r="C67" s="156" t="s">
         <v>68</v>
       </c>
-      <c r="D67" s="157"/>
+      <c r="D67" s="156"/>
       <c r="E67" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="F67" s="158" t="s">
+      <c r="F67" s="159" t="s">
         <v>66</v>
       </c>
-      <c r="G67" s="158"/>
-      <c r="H67" s="158"/>
+      <c r="G67" s="159"/>
+      <c r="H67" s="159"/>
       <c r="I67" s="35"/>
     </row>
     <row r="68" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="33"/>
-      <c r="C68" s="155" t="s">
+      <c r="C68" s="157" t="s">
         <v>67</v>
       </c>
-      <c r="D68" s="155"/>
+      <c r="D68" s="157"/>
       <c r="E68" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="F68" s="156" t="s">
+      <c r="F68" s="158" t="s">
         <v>66</v>
       </c>
-      <c r="G68" s="156"/>
-      <c r="H68" s="156"/>
+      <c r="G68" s="158"/>
+      <c r="H68" s="158"/>
       <c r="I68" s="35"/>
     </row>
     <row r="69" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7280,6 +7280,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="C64:H64"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="F67:H67"/>
     <mergeCell ref="D44:G44"/>
     <mergeCell ref="D57:G57"/>
     <mergeCell ref="D58:G58"/>
@@ -7293,13 +7300,6 @@
     <mergeCell ref="F47:H47"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="F48:H48"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="C64:H64"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="F67:H67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
20191120 - Added Run and QOL improvements
QOL: Gravity
Bullet caps
</commit_message>
<xml_diff>
--- a/res/references/First Platformer Checklist.xlsx
+++ b/res/references/First Platformer Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apauley\git\platforming101\res\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D097E5-6092-455E-9C03-12C37899D8D0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6549F6C-1D3D-4283-8294-13F49E229EA1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="1935" windowWidth="28695" windowHeight="11745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="Ba">'Phase 2'!$B$2</definedName>
     <definedName name="Bb">'Phase 2'!$B$12</definedName>
     <definedName name="Bc">'Phase 2'!$B$22</definedName>
-    <definedName name="Bd">'Phase 2'!$B$32</definedName>
+    <definedName name="Bd">'Phase 2'!$B$42</definedName>
     <definedName name="Ca">'Phase 3'!$B$2</definedName>
     <definedName name="Cb">'Phase 3'!$B$12</definedName>
     <definedName name="Cc">'Phase 3'!$B$22</definedName>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="70">
   <si>
     <t>Feature</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>Slot B</t>
+  </si>
+  <si>
+    <t>Player can run</t>
   </si>
 </sst>
 </file>
@@ -853,7 +856,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1061,12 +1064,27 @@
         <color indexed="64"/>
       </diagonal>
     </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal style="medium">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1303,6 +1321,16 @@
     <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1708,10 +1736,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1775,6 +1803,7 @@
       <c r="B5" s="4"/>
       <c r="C5" s="125"/>
       <c r="D5" s="129">
+        <f>D4+1</f>
         <v>1</v>
       </c>
       <c r="E5" s="130" t="s">
@@ -1790,6 +1819,7 @@
       <c r="B6" s="4"/>
       <c r="C6" s="125"/>
       <c r="D6" s="127">
+        <f t="shared" ref="D6:D8" si="0">D5+1</f>
         <v>2</v>
       </c>
       <c r="E6" s="126" t="s">
@@ -1805,6 +1835,7 @@
       <c r="B7" s="4"/>
       <c r="C7" s="125"/>
       <c r="D7" s="129">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E7" s="130" t="s">
@@ -1820,6 +1851,7 @@
       <c r="B8" s="4"/>
       <c r="C8" s="125"/>
       <c r="D8" s="132">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E8" s="133" t="s">
@@ -1841,7 +1873,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
-      <c r="B10" s="7"/>
+      <c r="B10" s="125"/>
       <c r="C10" s="144" t="s">
         <v>8</v>
       </c>
@@ -1855,6 +1887,7 @@
       <c r="B11" s="4"/>
       <c r="C11" s="125"/>
       <c r="D11" s="127">
+        <f>D8+1</f>
         <v>5</v>
       </c>
       <c r="E11" s="126" t="s">
@@ -1870,6 +1903,7 @@
       <c r="B12" s="4"/>
       <c r="C12" s="125"/>
       <c r="D12" s="129">
+        <f t="shared" ref="D12:D15" si="1">D11+1</f>
         <v>6</v>
       </c>
       <c r="E12" s="130" t="s">
@@ -1883,8 +1917,9 @@
     <row r="13" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="8"/>
+      <c r="C13" s="125"/>
       <c r="D13" s="127">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="E13" s="126" t="s">
@@ -1899,64 +1934,67 @@
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="125"/>
-      <c r="D14" s="139">
+      <c r="D14" s="129">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="E14" s="140" t="s">
+      <c r="E14" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="141" t="s">
-        <v>9</v>
+      <c r="F14" s="131" t="s">
+        <v>69</v>
       </c>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" ht="3.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="135"/>
-      <c r="E15" s="135"/>
-      <c r="F15" s="136"/>
+      <c r="C15" s="160"/>
+      <c r="D15" s="127">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="E15" s="126" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="128" t="s">
+        <v>9</v>
+      </c>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="3.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="145" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="161"/>
+      <c r="D16" s="162"/>
+      <c r="E16" s="162"/>
+      <c r="F16" s="163"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="145" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="143"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="127">
-        <v>9</v>
-      </c>
-      <c r="E17" s="126" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="128" t="s">
-        <v>11</v>
-      </c>
+      <c r="D17" s="142"/>
+      <c r="E17" s="142"/>
+      <c r="F17" s="143"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="129">
+      <c r="C18" s="9"/>
+      <c r="D18" s="127">
+        <f>D15+1</f>
         <v>10</v>
       </c>
-      <c r="E18" s="130" t="s">
+      <c r="E18" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="131" t="s">
-        <v>13</v>
+      <c r="F18" s="128" t="s">
+        <v>11</v>
       </c>
       <c r="G18" s="4"/>
     </row>
@@ -1964,14 +2002,15 @@
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
-      <c r="D19" s="127">
+      <c r="D19" s="129">
+        <f t="shared" ref="D19:D23" si="2">D18+1</f>
         <v>11</v>
       </c>
-      <c r="E19" s="126" t="s">
+      <c r="E19" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="128" t="s">
-        <v>12</v>
+      <c r="F19" s="131" t="s">
+        <v>13</v>
       </c>
       <c r="G19" s="4"/>
     </row>
@@ -1979,14 +2018,15 @@
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="129">
+      <c r="D20" s="127">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="E20" s="130" t="s">
+      <c r="E20" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="131" t="s">
-        <v>15</v>
+      <c r="F20" s="128" t="s">
+        <v>12</v>
       </c>
       <c r="G20" s="4"/>
     </row>
@@ -1994,14 +2034,15 @@
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="127">
+      <c r="D21" s="129">
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="E21" s="126" t="s">
+      <c r="E21" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F21" s="128" t="s">
-        <v>16</v>
+      <c r="F21" s="131" t="s">
+        <v>15</v>
       </c>
       <c r="G21" s="4"/>
     </row>
@@ -2009,64 +2050,67 @@
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
-      <c r="D22" s="132">
+      <c r="D22" s="127">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="E22" s="133" t="s">
+      <c r="E22" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="134" t="s">
-        <v>17</v>
+      <c r="F22" s="128" t="s">
+        <v>16</v>
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" ht="3.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="135"/>
-      <c r="E23" s="135"/>
-      <c r="F23" s="136"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="132">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="E23" s="133" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="134" t="s">
+        <v>17</v>
+      </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="3.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="144" t="s">
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="135"/>
+      <c r="E24" s="135"/>
+      <c r="F24" s="136"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="144" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="137"/>
-      <c r="E24" s="137"/>
-      <c r="F24" s="138"/>
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="127">
-        <v>15</v>
-      </c>
-      <c r="E25" s="126" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" s="128" t="s">
-        <v>19</v>
-      </c>
+      <c r="D25" s="137"/>
+      <c r="E25" s="137"/>
+      <c r="F25" s="138"/>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="129">
+      <c r="C26" s="9"/>
+      <c r="D26" s="127">
+        <f>D23+1</f>
         <v>16</v>
       </c>
-      <c r="E26" s="130" t="s">
+      <c r="E26" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="131" t="s">
-        <v>20</v>
+      <c r="F26" s="128" t="s">
+        <v>19</v>
       </c>
       <c r="G26" s="4"/>
     </row>
@@ -2074,14 +2118,15 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="127">
+      <c r="D27" s="129">
+        <f t="shared" ref="D27:D34" si="3">D26+1</f>
         <v>17</v>
       </c>
-      <c r="E27" s="126" t="s">
+      <c r="E27" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="128" t="s">
-        <v>21</v>
+      <c r="F27" s="131" t="s">
+        <v>20</v>
       </c>
       <c r="G27" s="4"/>
     </row>
@@ -2089,14 +2134,15 @@
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="129">
+      <c r="D28" s="127">
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="E28" s="130" t="s">
+      <c r="E28" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="131" t="s">
-        <v>22</v>
+      <c r="F28" s="128" t="s">
+        <v>21</v>
       </c>
       <c r="G28" s="4"/>
     </row>
@@ -2104,14 +2150,15 @@
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="127">
+      <c r="D29" s="129">
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="E29" s="126" t="s">
+      <c r="E29" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="128" t="s">
-        <v>23</v>
+      <c r="F29" s="131" t="s">
+        <v>22</v>
       </c>
       <c r="G29" s="4"/>
     </row>
@@ -2119,14 +2166,15 @@
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="129">
+      <c r="D30" s="127">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="E30" s="130" t="s">
+      <c r="E30" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="131" t="s">
-        <v>24</v>
+      <c r="F30" s="128" t="s">
+        <v>23</v>
       </c>
       <c r="G30" s="4"/>
     </row>
@@ -2134,14 +2182,15 @@
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="8"/>
-      <c r="D31" s="127">
+      <c r="D31" s="129">
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="E31" s="126" t="s">
+      <c r="E31" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="128" t="s">
-        <v>25</v>
+      <c r="F31" s="131" t="s">
+        <v>24</v>
       </c>
       <c r="G31" s="4"/>
     </row>
@@ -2150,13 +2199,14 @@
       <c r="B32" s="4"/>
       <c r="C32" s="8"/>
       <c r="D32" s="127">
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="E32" s="126" t="s">
         <v>35</v>
       </c>
       <c r="F32" s="128" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G32" s="4"/>
     </row>
@@ -2164,64 +2214,67 @@
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="139">
+      <c r="D33" s="127">
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="E33" s="140" t="s">
+      <c r="E33" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F33" s="141" t="s">
-        <v>48</v>
+      <c r="F33" s="128" t="s">
+        <v>26</v>
       </c>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" ht="3.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
-      <c r="C34" s="146"/>
-      <c r="D34" s="135"/>
-      <c r="E34" s="135"/>
-      <c r="F34" s="136"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="139">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="E34" s="140" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="141" t="s">
+        <v>48</v>
+      </c>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="3.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="145" t="s">
+      <c r="B35" s="4"/>
+      <c r="C35" s="146"/>
+      <c r="D35" s="135"/>
+      <c r="E35" s="135"/>
+      <c r="F35" s="136"/>
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="145" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="142"/>
-      <c r="E35" s="142"/>
-      <c r="F35" s="143"/>
-      <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="127">
-        <v>24</v>
-      </c>
-      <c r="E36" s="126" t="s">
-        <v>35</v>
-      </c>
-      <c r="F36" s="128" t="s">
-        <v>28</v>
-      </c>
+      <c r="D36" s="142"/>
+      <c r="E36" s="142"/>
+      <c r="F36" s="143"/>
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="129">
+      <c r="C37" s="9"/>
+      <c r="D37" s="127">
+        <f>D34+1</f>
         <v>25</v>
       </c>
-      <c r="E37" s="130" t="s">
+      <c r="E37" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F37" s="131" t="s">
-        <v>29</v>
+      <c r="F37" s="128" t="s">
+        <v>28</v>
       </c>
       <c r="G37" s="4"/>
     </row>
@@ -2229,14 +2282,15 @@
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="8"/>
-      <c r="D38" s="127">
+      <c r="D38" s="129">
+        <f t="shared" ref="D38:D44" si="4">D37+1</f>
         <v>26</v>
       </c>
-      <c r="E38" s="126" t="s">
+      <c r="E38" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F38" s="128" t="s">
-        <v>30</v>
+      <c r="F38" s="131" t="s">
+        <v>29</v>
       </c>
       <c r="G38" s="4"/>
     </row>
@@ -2244,14 +2298,15 @@
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="129">
+      <c r="D39" s="127">
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="E39" s="130" t="s">
+      <c r="E39" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F39" s="131" t="s">
-        <v>31</v>
+      <c r="F39" s="128" t="s">
+        <v>30</v>
       </c>
       <c r="G39" s="4"/>
     </row>
@@ -2259,14 +2314,15 @@
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="8"/>
-      <c r="D40" s="127">
+      <c r="D40" s="129">
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="E40" s="126" t="s">
+      <c r="E40" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F40" s="128" t="s">
-        <v>32</v>
+      <c r="F40" s="131" t="s">
+        <v>31</v>
       </c>
       <c r="G40" s="4"/>
     </row>
@@ -2274,14 +2330,15 @@
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="8"/>
-      <c r="D41" s="129">
+      <c r="D41" s="127">
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
-      <c r="E41" s="130" t="s">
+      <c r="E41" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F41" s="131" t="s">
-        <v>33</v>
+      <c r="F41" s="128" t="s">
+        <v>32</v>
       </c>
       <c r="G41" s="4"/>
     </row>
@@ -2289,14 +2346,15 @@
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="127">
+      <c r="D42" s="129">
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="E42" s="126" t="s">
+      <c r="E42" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F42" s="128" t="s">
-        <v>63</v>
+      <c r="F42" s="131" t="s">
+        <v>33</v>
       </c>
       <c r="G42" s="4"/>
     </row>
@@ -2304,25 +2362,42 @@
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="8"/>
-      <c r="D43" s="139">
+      <c r="D43" s="127">
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
-      <c r="E43" s="140" t="s">
+      <c r="E43" s="126" t="s">
         <v>35</v>
       </c>
-      <c r="F43" s="141" t="s">
-        <v>34</v>
+      <c r="F43" s="128" t="s">
+        <v>63</v>
       </c>
       <c r="G43" s="4"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="4"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="139">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="E44" s="140" t="s">
+        <v>35</v>
+      </c>
+      <c r="F44" s="141" t="s">
+        <v>34</v>
+      </c>
       <c r="G44" s="4"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2331,9 +2406,9 @@
   <hyperlinks>
     <hyperlink ref="C3:F3" location="'Phase 1'!A1" display="1 - Initialization" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="C10:F10" location="'Phase 2'!A1" display="2 - Movement" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C16:F16" location="'Phase 3'!A1" display="3 - Environment" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C24:F24" location="'Phase 4'!A1" display="4 - UI" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C35:F35" location="'Phase 5'!A1" display="5 - Advanced" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C17:F17" location="'Phase 3'!A1" display="3 - Environment" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C25:F25" location="'Phase 4'!A1" display="4 - UI" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C36:F36" location="'Phase 5'!A1" display="5 - Advanced" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="D4:F4" location="Onea" display="a" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="D5:F5" location="Ab" display="b" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="D6:F6" location="Ac" display="c" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
@@ -2342,31 +2417,31 @@
     <hyperlink ref="D11:F11" location="Ba" display="a" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="D12:F12" location="Bb" display="b" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="D13:F13" location="Bc" display="c" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="D14:F14" location="Bd" display="d" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="D17:F17" location="Ca" display="a" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D18:F18" location="Cb" display="b" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="D19:F19" location="Cc" display="c" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="D20:F20" location="Cd" display="d" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="D21:F21" location="Ce" display="e" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D22:F22" location="Cf" display="f" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="D25:F25" location="Da" display="a" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="D26:F26" location="Db" display="b" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="D27:F27" location="Dc" display="c" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D28:F28" location="Dd" display="d" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="D29:F29" location="De" display="e" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="D30:F30" location="Df" display="f" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="D31:F31" location="Dg" display="g" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D32:F32" location="Dh" display="h" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="D33:F33" location="Di" display="i" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="D36:F36" location="Ea" display="a" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="D37:F37" location="Eb" display="b" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="D38:F38" location="Ec" display="c" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="D39:F39" location="Ed" display="d" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="D40:F40" location="Ee" display="e" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="D41:F41" location="Ef" display="f" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="D42:F42" location="Eg" display="g" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="D43:F43" location="Eh" display="h" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="D15:F15" location="Bd" display="d" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D19:F19" location="Cb" display="b" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D20:F20" location="Cc" display="c" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D21:F21" location="Cd" display="d" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D22:F22" location="Ce" display="e" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D23:F23" location="Cf" display="f" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D27:F27" location="Db" display="b" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D28:F28" location="Dc" display="c" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D29:F29" location="Dd" display="d" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="D30:F30" location="De" display="e" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="D31:F31" location="Df" display="f" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="D32:F32" location="Dg" display="g" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D33:F33" location="Dh" display="h" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="D34:F34" location="Di" display="i" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="D38:F38" location="Eb" display="b" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="D39:F39" location="Ec" display="c" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="D40:F40" location="Ed" display="d" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="D41:F41" location="Ee" display="e" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="D42:F42" location="Ef" display="f" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="D43:F43" location="Eg" display="g" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="D44:F44" location="Eh" display="h" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
     <hyperlink ref="F4" location="Aa" display="Player spawns on screen" xr:uid="{737FFEE2-DFD5-42C6-B858-2FCEF8EC9F7D}"/>
+    <hyperlink ref="D18" location="Ba" display="a" xr:uid="{398B4FB7-3A48-473F-98F0-BC34A0A83F75}"/>
+    <hyperlink ref="D26" location="Ba" display="a" xr:uid="{EFDB2CFE-CC8D-43E9-8E35-81704B9DD70E}"/>
+    <hyperlink ref="D37" location="Ba" display="a" xr:uid="{93F0514F-0A15-4AA2-AE5C-F68C4F8FB0BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2380,14 +2455,15 @@
   </sheetPr>
   <dimension ref="B2:P50"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="W53" sqref="W53"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
+        <f>Checklist!D4</f>
         <v>0</v>
       </c>
       <c r="C2" t="str">
@@ -2539,6 +2615,7 @@
     </row>
     <row r="12" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
+        <f>B2+1</f>
         <v>1</v>
       </c>
       <c r="C12" t="str">
@@ -2632,6 +2709,7 @@
     </row>
     <row r="22" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
+        <f>B12+1</f>
         <v>2</v>
       </c>
       <c r="C22" t="str">
@@ -2747,6 +2825,7 @@
     </row>
     <row r="32" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1">
+        <f>B22+1</f>
         <v>3</v>
       </c>
       <c r="C32" t="str">
@@ -2862,6 +2941,7 @@
     </row>
     <row r="42" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="1">
+        <f>B32+1</f>
         <v>4</v>
       </c>
       <c r="C42" t="str">
@@ -2985,16 +3065,17 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FFFFF3CD"/>
   </sheetPr>
-  <dimension ref="B2:O40"/>
+  <dimension ref="B2:O50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
+        <f>'Phase 1'!B42+1</f>
         <v>5</v>
       </c>
       <c r="C2" t="str">
@@ -3110,6 +3191,7 @@
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
+        <f>B2+1</f>
         <v>6</v>
       </c>
       <c r="C12" t="str">
@@ -3225,6 +3307,7 @@
     </row>
     <row r="22" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
+        <f>B12+1</f>
         <v>7</v>
       </c>
       <c r="C22" t="str">
@@ -3342,143 +3425,260 @@
     </row>
     <row r="32" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1">
+        <f>B22+1</f>
         <v>8</v>
       </c>
       <c r="C32" t="str">
-        <f>Checklist!E14</f>
+        <f>Checklist!E41</f>
         <v>-</v>
       </c>
       <c r="D32" t="str">
         <f>Checklist!F14</f>
-        <v>Camera will follow player</v>
+        <v>Player can run</v>
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="39"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
       <c r="G33" s="40"/>
       <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="40"/>
-      <c r="L33" s="40"/>
-      <c r="M33" s="41"/>
-      <c r="N33" s="60"/>
+      <c r="I33" s="41"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="15"/>
+      <c r="B34" s="14"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
-      <c r="F34" s="14"/>
+      <c r="F34" s="15"/>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="15"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
       <c r="O34" s="12"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="15"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="42"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
       <c r="G35" s="43"/>
       <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
-      <c r="M35" s="44"/>
-      <c r="N35" s="17"/>
+      <c r="I35" s="44"/>
       <c r="O35" s="12"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="15"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="15"/>
       <c r="G36" s="15"/>
       <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="43"/>
-      <c r="M36" s="44"/>
-      <c r="N36" s="17"/>
+      <c r="I36" s="44"/>
       <c r="O36" s="12"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="15"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="42"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
       <c r="G37" s="43"/>
       <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="43"/>
-      <c r="M37" s="44"/>
-      <c r="N37" s="17"/>
+      <c r="I37" s="44"/>
       <c r="O37" s="12"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="15"/>
-      <c r="C38" s="17"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="43"/>
       <c r="D38" s="15"/>
       <c r="E38" s="15"/>
-      <c r="F38" s="42"/>
+      <c r="F38" s="43"/>
       <c r="G38" s="43"/>
       <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="16"/>
-      <c r="N38" s="15"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
       <c r="O38" s="12"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B39" s="15"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="42"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="107"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="57"/>
       <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="43"/>
-      <c r="L39" s="43"/>
-      <c r="M39" s="44"/>
-      <c r="N39" s="17"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="44"/>
       <c r="O39" s="12"/>
     </row>
     <row r="40" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="19"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
       <c r="G40" s="20"/>
       <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
-      <c r="M40" s="21"/>
-      <c r="N40" s="15"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="12"/>
+      <c r="N40" s="12"/>
       <c r="O40" s="12"/>
+    </row>
+    <row r="42" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="1">
+        <f>B32+1</f>
+        <v>9</v>
+      </c>
+      <c r="C42" t="str">
+        <f>Checklist!E15</f>
+        <v>-</v>
+      </c>
+      <c r="D42" t="str">
+        <f>Checklist!F15</f>
+        <v>Camera will follow player</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="40"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
+      <c r="K43" s="40"/>
+      <c r="L43" s="40"/>
+      <c r="M43" s="41"/>
+      <c r="N43" s="60"/>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="16"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="12"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B45" s="15"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="43"/>
+      <c r="M45" s="44"/>
+      <c r="N45" s="17"/>
+      <c r="O45" s="12"/>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B46" s="15"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="43"/>
+      <c r="M46" s="44"/>
+      <c r="N46" s="17"/>
+      <c r="O46" s="12"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B47" s="15"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="42"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="43"/>
+      <c r="J47" s="43"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="43"/>
+      <c r="M47" s="44"/>
+      <c r="N47" s="17"/>
+      <c r="O47" s="12"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B48" s="15"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="16"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="12"/>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" s="15"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="43"/>
+      <c r="I49" s="30"/>
+      <c r="J49" s="43"/>
+      <c r="K49" s="43"/>
+      <c r="L49" s="43"/>
+      <c r="M49" s="44"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="12"/>
+    </row>
+    <row r="50" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="15"/>
+      <c r="O50" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3492,20 +3692,23 @@
   </sheetPr>
   <dimension ref="B2:O60"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
-        <v>9</v>
+        <f>'Phase 2'!B42+1</f>
+        <v>10</v>
       </c>
       <c r="C2" t="str">
-        <f>Checklist!E17</f>
+        <f>Checklist!E18</f>
         <v>-</v>
       </c>
       <c r="D2" t="str">
-        <f>Checklist!F17</f>
+        <f>Checklist!F18</f>
         <v>Enemies spawn</v>
       </c>
     </row>
@@ -3615,14 +3818,15 @@
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
-        <v>10</v>
+        <f>B2+1</f>
+        <v>11</v>
       </c>
       <c r="C12" t="str">
-        <f>Checklist!E18</f>
+        <f>Checklist!E19</f>
         <v>-</v>
       </c>
       <c r="D12" t="str">
-        <f>Checklist!F18</f>
+        <f>Checklist!F19</f>
         <v>Enemies collide with environment</v>
       </c>
     </row>
@@ -3735,11 +3939,11 @@
         <v>11</v>
       </c>
       <c r="C22" t="str">
-        <f>Checklist!E19</f>
+        <f>Checklist!E20</f>
         <v>-</v>
       </c>
       <c r="D22" t="str">
-        <f>Checklist!F19</f>
+        <f>Checklist!F20</f>
         <v>Enemies move</v>
       </c>
     </row>
@@ -3854,11 +4058,11 @@
         <v>12</v>
       </c>
       <c r="C32" t="str">
-        <f>Checklist!E20</f>
+        <f>Checklist!E21</f>
         <v>-</v>
       </c>
       <c r="D32" t="str">
-        <f>Checklist!F20</f>
+        <f>Checklist!F21</f>
         <v>Enemies collide with player</v>
       </c>
     </row>
@@ -3969,11 +4173,11 @@
         <v>13</v>
       </c>
       <c r="C42" t="str">
-        <f>Checklist!E21</f>
+        <f>Checklist!E22</f>
         <v>-</v>
       </c>
       <c r="D42" t="str">
-        <f>Checklist!F21</f>
+        <f>Checklist!F22</f>
         <v>Enemies shoot</v>
       </c>
     </row>
@@ -4085,11 +4289,11 @@
         <v>14</v>
       </c>
       <c r="C52" t="str">
-        <f>Checklist!E22</f>
+        <f>Checklist!E23</f>
         <v>-</v>
       </c>
       <c r="D52" t="str">
-        <f>Checklist!F22</f>
+        <f>Checklist!F23</f>
         <v>Shots collide with player/enemies</v>
       </c>
     </row>
@@ -4208,22 +4412,23 @@
   </sheetPr>
   <dimension ref="B2:X96"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
+        <f>'Phase 3'!B52+1</f>
         <v>15</v>
       </c>
       <c r="C2" t="str">
-        <f>Checklist!E25</f>
+        <f>Checklist!E26</f>
         <v>-</v>
       </c>
       <c r="D2" t="str">
-        <f>Checklist!F25</f>
+        <f>Checklist!F26</f>
         <v>Bullets tracked</v>
       </c>
     </row>
@@ -4337,14 +4542,15 @@
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
+        <f>B2+1</f>
         <v>16</v>
       </c>
       <c r="C12" t="str">
-        <f>Checklist!E26</f>
+        <f>Checklist!E27</f>
         <v>-</v>
       </c>
       <c r="D12" t="str">
-        <f>Checklist!F26</f>
+        <f>Checklist!F27</f>
         <v>Reload implemented</v>
       </c>
     </row>
@@ -4459,14 +4665,15 @@
     </row>
     <row r="22" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
+        <f>B12+1</f>
         <v>17</v>
       </c>
       <c r="C22" t="str">
-        <f>Checklist!E27</f>
+        <f>Checklist!E28</f>
         <v>-</v>
       </c>
       <c r="D22" t="str">
-        <f>Checklist!F27</f>
+        <f>Checklist!F28</f>
         <v>Score tracked (kills, time elapsed, etc.)</v>
       </c>
     </row>
@@ -4580,14 +4787,15 @@
     </row>
     <row r="32" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1">
+        <f>B22+1</f>
         <v>18</v>
       </c>
       <c r="C32" t="str">
-        <f>Checklist!E28</f>
+        <f>Checklist!E29</f>
         <v>-</v>
       </c>
       <c r="D32" t="str">
-        <f>Checklist!F28</f>
+        <f>Checklist!F29</f>
         <v>Pause button (stop time)</v>
       </c>
     </row>
@@ -4702,14 +4910,15 @@
     </row>
     <row r="42" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="1">
+        <f>B32+1</f>
         <v>19</v>
       </c>
       <c r="C42" t="str">
-        <f>Checklist!E29</f>
+        <f>Checklist!E30</f>
         <v>-</v>
       </c>
       <c r="D42" t="str">
-        <f>Checklist!F29</f>
+        <f>Checklist!F30</f>
         <v>Menu screen (utilizes pause button)</v>
       </c>
     </row>
@@ -4830,14 +5039,15 @@
     </row>
     <row r="52" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="1">
+        <f>B42+1</f>
         <v>20</v>
       </c>
       <c r="C52" t="str">
-        <f>Checklist!E30</f>
+        <f>Checklist!E31</f>
         <v>-</v>
       </c>
       <c r="D52" t="str">
-        <f>Checklist!F30</f>
+        <f>Checklist!F31</f>
         <v>Slow Time (death scene)</v>
       </c>
     </row>
@@ -4951,14 +5161,15 @@
     </row>
     <row r="62" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="1">
+        <f>B52+1</f>
         <v>21</v>
       </c>
       <c r="C62" t="str">
-        <f>Checklist!E31</f>
+        <f>Checklist!E32</f>
         <v>-</v>
       </c>
       <c r="D62" t="str">
-        <f>Checklist!F31</f>
+        <f>Checklist!F32</f>
         <v>Death Screen</v>
       </c>
     </row>
@@ -5080,14 +5291,15 @@
     </row>
     <row r="72" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="1">
+        <f>B62+1</f>
         <v>22</v>
       </c>
       <c r="C72" t="str">
-        <f>Checklist!E32</f>
+        <f>Checklist!E33</f>
         <v>-</v>
       </c>
       <c r="D72" t="str">
-        <f>Checklist!F32</f>
+        <f>Checklist!F33</f>
         <v>Zoom in (no idea how to do this)</v>
       </c>
     </row>
@@ -5225,14 +5437,15 @@
     </row>
     <row r="82" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="1">
+        <f>B72+1</f>
         <v>23</v>
       </c>
       <c r="C82" t="str">
-        <f>Checklist!E33</f>
+        <f>Checklist!E34</f>
         <v>-</v>
       </c>
       <c r="D82" t="str">
-        <f>Checklist!F33</f>
+        <f>Checklist!F34</f>
         <v>Zoom out (no idea how to do this)</v>
       </c>
     </row>
@@ -5511,8 +5724,8 @@
   </sheetPr>
   <dimension ref="B2:AA106"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="AA70" sqref="AA70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5522,14 +5735,15 @@
   <sheetData>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
+        <f>'Phase 4'!B82+1</f>
         <v>24</v>
       </c>
       <c r="C2" t="str">
-        <f>Checklist!E36</f>
+        <f>Checklist!E37</f>
         <v>-</v>
       </c>
       <c r="D2" t="str">
-        <f>Checklist!F36</f>
+        <f>Checklist!F37</f>
         <v>New level after x enemies killed</v>
       </c>
     </row>
@@ -5661,14 +5875,15 @@
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
+        <f>B2+1</f>
         <v>25</v>
       </c>
       <c r="C12" t="str">
-        <f>Checklist!E37</f>
+        <f>Checklist!E38</f>
         <v>-</v>
       </c>
       <c r="D12" t="str">
-        <f>Checklist!F37</f>
+        <f>Checklist!F38</f>
         <v>Spawn harder enemies</v>
       </c>
     </row>
@@ -5800,14 +6015,15 @@
     </row>
     <row r="22" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
+        <f>B12+1</f>
         <v>26</v>
       </c>
       <c r="C22" t="str">
-        <f>Checklist!E38</f>
+        <f>Checklist!E39</f>
         <v>-</v>
       </c>
       <c r="D22" t="str">
-        <f>Checklist!F38</f>
+        <f>Checklist!F39</f>
         <v>Random drops (health, items, weapons)</v>
       </c>
     </row>
@@ -5945,14 +6161,15 @@
     </row>
     <row r="32" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1">
+        <f>B22+1</f>
         <v>27</v>
       </c>
       <c r="C32" t="str">
-        <f>Checklist!E39</f>
+        <f>Checklist!E40</f>
         <v>-</v>
       </c>
       <c r="D32" t="str">
-        <f>Checklist!F39</f>
+        <f>Checklist!F40</f>
         <v>Special abilities</v>
       </c>
     </row>
@@ -6088,14 +6305,15 @@
     </row>
     <row r="42" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="1">
+        <f>B32+1</f>
         <v>28</v>
       </c>
       <c r="C42" t="str">
-        <f>Checklist!E40</f>
+        <f>Checklist!E41</f>
         <v>-</v>
       </c>
       <c r="D42" t="str">
-        <f>Checklist!F40</f>
+        <f>Checklist!F41</f>
         <v>High score chart</v>
       </c>
     </row>
@@ -6207,14 +6425,15 @@
     </row>
     <row r="52" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="1">
+        <f>B42+1</f>
         <v>29</v>
       </c>
       <c r="C52" t="str">
-        <f>Checklist!E41</f>
+        <f>Checklist!E42</f>
         <v>-</v>
       </c>
       <c r="D52" t="str">
-        <f>Checklist!F41</f>
+        <f>Checklist!F42</f>
         <v>Save game</v>
       </c>
     </row>
@@ -6356,14 +6575,15 @@
     </row>
     <row r="62" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="1">
+        <f>B52+1</f>
         <v>30</v>
       </c>
       <c r="C62" t="str">
-        <f>Checklist!E42</f>
+        <f>Checklist!E43</f>
         <v>-</v>
       </c>
       <c r="D62" t="str">
-        <f>Checklist!F42</f>
+        <f>Checklist!F43</f>
         <v>Continue game</v>
       </c>
     </row>
@@ -6469,14 +6689,15 @@
     </row>
     <row r="72" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="1">
+        <f>B62+1</f>
         <v>31</v>
       </c>
       <c r="C72" t="str">
-        <f>Checklist!E43</f>
+        <f>Checklist!E44</f>
         <v>-</v>
       </c>
       <c r="D72" t="str">
-        <f>Checklist!F43</f>
+        <f>Checklist!F44</f>
         <v>Replay (track player movement…oh my!)</v>
       </c>
     </row>

</xml_diff>

<commit_message>
20191121 - Up Through Enemies Collide With Player Implemented
</commit_message>
<xml_diff>
--- a/res/references/First Platformer Checklist.xlsx
+++ b/res/references/First Platformer Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apauley\git\platforming101\res\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6549F6C-1D3D-4283-8294-13F49E229EA1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917F76CF-4D68-48FF-8181-99436C447F98}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1282,6 +1282,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1306,31 +1316,21 @@
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1739,7 +1739,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1763,13 +1763,13 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="147" t="s">
+      <c r="B2" s="151" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
-      <c r="F2" s="149"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="153"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1949,7 +1949,7 @@
     <row r="15" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="160"/>
+      <c r="C15" s="147"/>
       <c r="D15" s="127">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1965,10 +1965,10 @@
     <row r="16" spans="1:7" ht="3.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="161"/>
-      <c r="D16" s="162"/>
-      <c r="E16" s="162"/>
-      <c r="F16" s="163"/>
+      <c r="C16" s="148"/>
+      <c r="D16" s="149"/>
+      <c r="E16" s="149"/>
+      <c r="F16" s="150"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1985,7 +1985,7 @@
     <row r="18" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="9"/>
+      <c r="C18" s="147"/>
       <c r="D18" s="127">
         <f>D15+1</f>
         <v>10</v>
@@ -2001,7 +2001,7 @@
     <row r="19" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="8"/>
+      <c r="C19" s="147"/>
       <c r="D19" s="129">
         <f t="shared" ref="D19:D23" si="2">D18+1</f>
         <v>11</v>
@@ -2017,7 +2017,7 @@
     <row r="20" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="8"/>
+      <c r="C20" s="147"/>
       <c r="D20" s="127">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -2033,7 +2033,7 @@
     <row r="21" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="8"/>
+      <c r="C21" s="147"/>
       <c r="D21" s="129">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -4955,12 +4955,12 @@
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="70"/>
       <c r="C45" s="77"/>
-      <c r="D45" s="150" t="s">
+      <c r="D45" s="154" t="s">
         <v>41</v>
       </c>
-      <c r="E45" s="150"/>
-      <c r="F45" s="150"/>
-      <c r="G45" s="150"/>
+      <c r="E45" s="154"/>
+      <c r="F45" s="154"/>
+      <c r="G45" s="154"/>
       <c r="H45" s="77"/>
       <c r="I45" s="56"/>
       <c r="O45" s="12"/>
@@ -4968,12 +4968,12 @@
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="70"/>
       <c r="C46" s="77"/>
-      <c r="D46" s="151" t="s">
+      <c r="D46" s="155" t="s">
         <v>42</v>
       </c>
-      <c r="E46" s="152"/>
-      <c r="F46" s="152"/>
-      <c r="G46" s="152"/>
+      <c r="E46" s="156"/>
+      <c r="F46" s="156"/>
+      <c r="G46" s="156"/>
       <c r="H46" s="77"/>
       <c r="I46" s="56"/>
       <c r="O46" s="12"/>
@@ -4981,12 +4981,12 @@
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="70"/>
       <c r="C47" s="77"/>
-      <c r="D47" s="154" t="s">
+      <c r="D47" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="E47" s="154"/>
-      <c r="F47" s="154"/>
-      <c r="G47" s="154"/>
+      <c r="E47" s="158"/>
+      <c r="F47" s="158"/>
+      <c r="G47" s="158"/>
       <c r="H47" s="77"/>
       <c r="I47" s="56"/>
       <c r="N47" s="61"/>
@@ -4995,12 +4995,12 @@
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="70"/>
       <c r="C48" s="77"/>
-      <c r="D48" s="151" t="s">
+      <c r="D48" s="155" t="s">
         <v>43</v>
       </c>
-      <c r="E48" s="151"/>
-      <c r="F48" s="151"/>
-      <c r="G48" s="151"/>
+      <c r="E48" s="155"/>
+      <c r="F48" s="155"/>
+      <c r="G48" s="155"/>
       <c r="H48" s="77"/>
       <c r="I48" s="75"/>
       <c r="J48" s="12"/>
@@ -5205,26 +5205,26 @@
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B65" s="70"/>
-      <c r="C65" s="153" t="s">
+      <c r="C65" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="D65" s="153"/>
-      <c r="E65" s="153"/>
-      <c r="F65" s="153"/>
-      <c r="G65" s="153"/>
-      <c r="H65" s="153"/>
+      <c r="D65" s="157"/>
+      <c r="E65" s="157"/>
+      <c r="F65" s="157"/>
+      <c r="G65" s="157"/>
+      <c r="H65" s="157"/>
       <c r="I65" s="56"/>
       <c r="O65" s="12"/>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="70"/>
       <c r="C66" s="77"/>
-      <c r="D66" s="150" t="s">
+      <c r="D66" s="154" t="s">
         <v>45</v>
       </c>
-      <c r="E66" s="150"/>
-      <c r="F66" s="150"/>
-      <c r="G66" s="150"/>
+      <c r="E66" s="154"/>
+      <c r="F66" s="154"/>
+      <c r="G66" s="154"/>
       <c r="H66" s="77"/>
       <c r="I66" s="56"/>
       <c r="O66" s="12"/>
@@ -5232,12 +5232,12 @@
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B67" s="70"/>
       <c r="C67" s="77"/>
-      <c r="D67" s="151" t="s">
+      <c r="D67" s="155" t="s">
         <v>46</v>
       </c>
-      <c r="E67" s="152"/>
-      <c r="F67" s="152"/>
-      <c r="G67" s="152"/>
+      <c r="E67" s="156"/>
+      <c r="F67" s="156"/>
+      <c r="G67" s="156"/>
       <c r="H67" s="77"/>
       <c r="I67" s="56"/>
       <c r="N67" s="29"/>
@@ -5246,12 +5246,12 @@
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B68" s="70"/>
       <c r="C68" s="77"/>
-      <c r="D68" s="151" t="s">
+      <c r="D68" s="155" t="s">
         <v>43</v>
       </c>
-      <c r="E68" s="151"/>
-      <c r="F68" s="151"/>
-      <c r="G68" s="151"/>
+      <c r="E68" s="155"/>
+      <c r="F68" s="155"/>
+      <c r="G68" s="155"/>
       <c r="H68" s="77"/>
       <c r="I68" s="56"/>
       <c r="J68" s="12"/>
@@ -6330,77 +6330,77 @@
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="33"/>
       <c r="C44" s="77"/>
-      <c r="D44" s="155" t="s">
+      <c r="D44" s="163" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="155"/>
-      <c r="F44" s="155"/>
-      <c r="G44" s="155"/>
+      <c r="E44" s="163"/>
+      <c r="F44" s="163"/>
+      <c r="G44" s="163"/>
       <c r="H44" s="77"/>
       <c r="I44" s="35"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="33"/>
-      <c r="C45" s="156" t="s">
+      <c r="C45" s="161" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="156"/>
+      <c r="D45" s="161"/>
       <c r="E45" s="121" t="s">
         <v>54</v>
       </c>
-      <c r="F45" s="156">
+      <c r="F45" s="161">
         <v>9001</v>
       </c>
-      <c r="G45" s="156"/>
-      <c r="H45" s="156"/>
+      <c r="G45" s="161"/>
+      <c r="H45" s="161"/>
       <c r="I45" s="35"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="33"/>
-      <c r="C46" s="157" t="s">
+      <c r="C46" s="159" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="157"/>
+      <c r="D46" s="159"/>
       <c r="E46" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="F46" s="157">
+      <c r="F46" s="159">
         <v>8999</v>
       </c>
-      <c r="G46" s="157"/>
-      <c r="H46" s="157"/>
+      <c r="G46" s="159"/>
+      <c r="H46" s="159"/>
       <c r="I46" s="35"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="33"/>
-      <c r="C47" s="157" t="s">
+      <c r="C47" s="159" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="157"/>
+      <c r="D47" s="159"/>
       <c r="E47" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="F47" s="157">
+      <c r="F47" s="159">
         <v>1337</v>
       </c>
-      <c r="G47" s="157"/>
-      <c r="H47" s="157"/>
+      <c r="G47" s="159"/>
+      <c r="H47" s="159"/>
       <c r="I47" s="35"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="33"/>
-      <c r="C48" s="157" t="s">
+      <c r="C48" s="159" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="157"/>
+      <c r="D48" s="159"/>
       <c r="E48" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="F48" s="157">
+      <c r="F48" s="159">
         <v>-5</v>
       </c>
-      <c r="G48" s="157"/>
-      <c r="H48" s="157"/>
+      <c r="G48" s="159"/>
+      <c r="H48" s="159"/>
       <c r="I48" s="35"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
@@ -6470,12 +6470,12 @@
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="90"/>
       <c r="C55" s="77"/>
-      <c r="D55" s="150" t="s">
+      <c r="D55" s="154" t="s">
         <v>41</v>
       </c>
-      <c r="E55" s="150"/>
-      <c r="F55" s="150"/>
-      <c r="G55" s="150"/>
+      <c r="E55" s="154"/>
+      <c r="F55" s="154"/>
+      <c r="G55" s="154"/>
       <c r="H55" s="77"/>
       <c r="I55" s="82"/>
       <c r="J55" s="83"/>
@@ -6488,12 +6488,12 @@
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" s="90"/>
       <c r="C56" s="77"/>
-      <c r="D56" s="151" t="s">
+      <c r="D56" s="155" t="s">
         <v>42</v>
       </c>
-      <c r="E56" s="152"/>
-      <c r="F56" s="152"/>
-      <c r="G56" s="152"/>
+      <c r="E56" s="156"/>
+      <c r="F56" s="156"/>
+      <c r="G56" s="156"/>
       <c r="H56" s="77"/>
       <c r="I56" s="82"/>
       <c r="J56" s="83"/>
@@ -6506,12 +6506,12 @@
     <row r="57" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="90"/>
       <c r="C57" s="77"/>
-      <c r="D57" s="151" t="s">
+      <c r="D57" s="155" t="s">
         <v>44</v>
       </c>
-      <c r="E57" s="152"/>
-      <c r="F57" s="152"/>
-      <c r="G57" s="152"/>
+      <c r="E57" s="156"/>
+      <c r="F57" s="156"/>
+      <c r="G57" s="156"/>
       <c r="H57" s="77"/>
       <c r="I57" s="82"/>
       <c r="J57" s="83"/>
@@ -6524,12 +6524,12 @@
     <row r="58" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="90"/>
       <c r="C58" s="77"/>
-      <c r="D58" s="154" t="s">
+      <c r="D58" s="158" t="s">
         <v>60</v>
       </c>
-      <c r="E58" s="154"/>
-      <c r="F58" s="154"/>
-      <c r="G58" s="154"/>
+      <c r="E58" s="158"/>
+      <c r="F58" s="158"/>
+      <c r="G58" s="158"/>
       <c r="H58" s="77"/>
       <c r="I58" s="89"/>
       <c r="J58" s="87"/>
@@ -6599,14 +6599,14 @@
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B64" s="33"/>
-      <c r="C64" s="150" t="s">
+      <c r="C64" s="154" t="s">
         <v>64</v>
       </c>
-      <c r="D64" s="150"/>
-      <c r="E64" s="150"/>
-      <c r="F64" s="150"/>
-      <c r="G64" s="150"/>
-      <c r="H64" s="150"/>
+      <c r="D64" s="154"/>
+      <c r="E64" s="154"/>
+      <c r="F64" s="154"/>
+      <c r="G64" s="154"/>
+      <c r="H64" s="154"/>
       <c r="I64" s="35"/>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
@@ -6621,50 +6621,50 @@
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="33"/>
-      <c r="C66" s="157" t="s">
+      <c r="C66" s="159" t="s">
         <v>65</v>
       </c>
-      <c r="D66" s="157"/>
+      <c r="D66" s="159"/>
       <c r="E66" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="F66" s="158" t="s">
+      <c r="F66" s="160" t="s">
         <v>66</v>
       </c>
-      <c r="G66" s="158"/>
-      <c r="H66" s="158"/>
+      <c r="G66" s="160"/>
+      <c r="H66" s="160"/>
       <c r="I66" s="35"/>
     </row>
     <row r="67" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="33"/>
-      <c r="C67" s="156" t="s">
+      <c r="C67" s="161" t="s">
         <v>68</v>
       </c>
-      <c r="D67" s="156"/>
+      <c r="D67" s="161"/>
       <c r="E67" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="F67" s="159" t="s">
+      <c r="F67" s="162" t="s">
         <v>66</v>
       </c>
-      <c r="G67" s="159"/>
-      <c r="H67" s="159"/>
+      <c r="G67" s="162"/>
+      <c r="H67" s="162"/>
       <c r="I67" s="35"/>
     </row>
     <row r="68" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="33"/>
-      <c r="C68" s="157" t="s">
+      <c r="C68" s="159" t="s">
         <v>67</v>
       </c>
-      <c r="D68" s="157"/>
+      <c r="D68" s="159"/>
       <c r="E68" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="F68" s="158" t="s">
+      <c r="F68" s="160" t="s">
         <v>66</v>
       </c>
-      <c r="G68" s="158"/>
-      <c r="H68" s="158"/>
+      <c r="G68" s="160"/>
+      <c r="H68" s="160"/>
       <c r="I68" s="35"/>
     </row>
     <row r="69" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7501,13 +7501,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="C64:H64"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="F67:H67"/>
     <mergeCell ref="D44:G44"/>
     <mergeCell ref="D57:G57"/>
     <mergeCell ref="D58:G58"/>
@@ -7521,6 +7514,13 @@
     <mergeCell ref="F47:H47"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="F48:H48"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="C64:H64"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="F67:H67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
20191122 - Tweaked Entity Collision Added Name/Group/FullName/ID
</commit_message>
<xml_diff>
--- a/res/references/First Platformer Checklist.xlsx
+++ b/res/references/First Platformer Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apauley\git\platforming101\res\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0819703F-0F70-4BC6-91EB-87519357576A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E64DA0-CDC0-44F9-B7CB-81203AEA3A5E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="72">
   <si>
     <t>Feature</t>
   </si>
@@ -342,6 +342,12 @@
   </si>
   <si>
     <t>Player can run</t>
+  </si>
+  <si>
+    <t>Add Sound Effects</t>
+  </si>
+  <si>
+    <t>Add Music</t>
   </si>
 </sst>
 </file>
@@ -1332,19 +1338,19 @@
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1752,10 +1758,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2299,7 +2305,7 @@
       <c r="B38" s="4"/>
       <c r="C38" s="7"/>
       <c r="D38" s="135">
-        <f t="shared" ref="D38:D44" si="4">D37+1</f>
+        <f t="shared" ref="D38:D46" si="4">D37+1</f>
         <v>26</v>
       </c>
       <c r="E38" s="136" t="s">
@@ -2394,26 +2400,46 @@
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="7"/>
-      <c r="D44" s="147">
+      <c r="D44" s="135">
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
-      <c r="E44" s="148" t="s">
+      <c r="E44" s="136" t="s">
         <v>35</v>
       </c>
-      <c r="F44" s="149" t="s">
+      <c r="F44" s="137" t="s">
         <v>34</v>
       </c>
       <c r="G44" s="4"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="128"/>
-      <c r="E45" s="128"/>
-      <c r="F45" s="129"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="132">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="E45" s="133" t="s">
+        <v>35</v>
+      </c>
+      <c r="F45" s="134" t="s">
+        <v>70</v>
+      </c>
       <c r="G45" s="4"/>
+    </row>
+    <row r="46" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="7"/>
+      <c r="D46" s="147">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+      <c r="E46" s="148" t="s">
+        <v>35</v>
+      </c>
+      <c r="F46" s="149" t="s">
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2458,6 +2484,8 @@
     <hyperlink ref="D18" location="Ba" display="a" xr:uid="{398B4FB7-3A48-473F-98F0-BC34A0A83F75}"/>
     <hyperlink ref="D26" location="Ba" display="a" xr:uid="{EFDB2CFE-CC8D-43E9-8E35-81704B9DD70E}"/>
     <hyperlink ref="D37" location="Ba" display="a" xr:uid="{93F0514F-0A15-4AA2-AE5C-F68C4F8FB0BE}"/>
+    <hyperlink ref="D45:F45" location="Eg" display="g" xr:uid="{4972F980-79FD-4AE3-92A1-794E254C95D3}"/>
+    <hyperlink ref="D46:F46" location="Eh" display="h" xr:uid="{FBFDCAC7-88B0-4B95-B4C4-2A42E51FD61D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3708,7 +3736,7 @@
   </sheetPr>
   <dimension ref="B2:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="AB48" sqref="AB48"/>
     </sheetView>
   </sheetViews>
@@ -6346,77 +6374,77 @@
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="32"/>
       <c r="C44" s="76"/>
-      <c r="D44" s="164" t="s">
+      <c r="D44" s="160" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="164"/>
-      <c r="F44" s="164"/>
-      <c r="G44" s="164"/>
+      <c r="E44" s="160"/>
+      <c r="F44" s="160"/>
+      <c r="G44" s="160"/>
       <c r="H44" s="76"/>
       <c r="I44" s="34"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="32"/>
-      <c r="C45" s="162" t="s">
+      <c r="C45" s="161" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="162"/>
+      <c r="D45" s="161"/>
       <c r="E45" s="120" t="s">
         <v>54</v>
       </c>
-      <c r="F45" s="162">
+      <c r="F45" s="161">
         <v>9001</v>
       </c>
-      <c r="G45" s="162"/>
-      <c r="H45" s="162"/>
+      <c r="G45" s="161"/>
+      <c r="H45" s="161"/>
       <c r="I45" s="34"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="32"/>
-      <c r="C46" s="160" t="s">
+      <c r="C46" s="162" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="160"/>
+      <c r="D46" s="162"/>
       <c r="E46" s="121" t="s">
         <v>54</v>
       </c>
-      <c r="F46" s="160">
+      <c r="F46" s="162">
         <v>8999</v>
       </c>
-      <c r="G46" s="160"/>
-      <c r="H46" s="160"/>
+      <c r="G46" s="162"/>
+      <c r="H46" s="162"/>
       <c r="I46" s="34"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="32"/>
-      <c r="C47" s="160" t="s">
+      <c r="C47" s="162" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="160"/>
+      <c r="D47" s="162"/>
       <c r="E47" s="121" t="s">
         <v>54</v>
       </c>
-      <c r="F47" s="160">
+      <c r="F47" s="162">
         <v>1337</v>
       </c>
-      <c r="G47" s="160"/>
-      <c r="H47" s="160"/>
+      <c r="G47" s="162"/>
+      <c r="H47" s="162"/>
       <c r="I47" s="34"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="32"/>
-      <c r="C48" s="160" t="s">
+      <c r="C48" s="162" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="160"/>
+      <c r="D48" s="162"/>
       <c r="E48" s="121" t="s">
         <v>54</v>
       </c>
-      <c r="F48" s="160">
+      <c r="F48" s="162">
         <v>-5</v>
       </c>
-      <c r="G48" s="160"/>
-      <c r="H48" s="160"/>
+      <c r="G48" s="162"/>
+      <c r="H48" s="162"/>
       <c r="I48" s="34"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
@@ -6637,50 +6665,50 @@
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="32"/>
-      <c r="C66" s="160" t="s">
+      <c r="C66" s="162" t="s">
         <v>65</v>
       </c>
-      <c r="D66" s="160"/>
+      <c r="D66" s="162"/>
       <c r="E66" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="F66" s="161" t="s">
+      <c r="F66" s="163" t="s">
         <v>66</v>
       </c>
-      <c r="G66" s="161"/>
-      <c r="H66" s="161"/>
+      <c r="G66" s="163"/>
+      <c r="H66" s="163"/>
       <c r="I66" s="34"/>
     </row>
     <row r="67" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="32"/>
-      <c r="C67" s="162" t="s">
+      <c r="C67" s="161" t="s">
         <v>68</v>
       </c>
-      <c r="D67" s="162"/>
+      <c r="D67" s="161"/>
       <c r="E67" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="F67" s="163" t="s">
+      <c r="F67" s="164" t="s">
         <v>66</v>
       </c>
-      <c r="G67" s="163"/>
-      <c r="H67" s="163"/>
+      <c r="G67" s="164"/>
+      <c r="H67" s="164"/>
       <c r="I67" s="34"/>
     </row>
     <row r="68" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="32"/>
-      <c r="C68" s="160" t="s">
+      <c r="C68" s="162" t="s">
         <v>67</v>
       </c>
-      <c r="D68" s="160"/>
+      <c r="D68" s="162"/>
       <c r="E68" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="F68" s="161" t="s">
+      <c r="F68" s="163" t="s">
         <v>66</v>
       </c>
-      <c r="G68" s="161"/>
-      <c r="H68" s="161"/>
+      <c r="G68" s="163"/>
+      <c r="H68" s="163"/>
       <c r="I68" s="34"/>
     </row>
     <row r="69" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7517,6 +7545,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="C64:H64"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="F67:H67"/>
     <mergeCell ref="D44:G44"/>
     <mergeCell ref="D57:G57"/>
     <mergeCell ref="D58:G58"/>
@@ -7530,13 +7565,6 @@
     <mergeCell ref="F47:H47"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="F48:H48"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="C64:H64"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="F67:H67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
20191125 - Bullets Tracked (Started)
Needs to be moved/handled differently...
</commit_message>
<xml_diff>
--- a/res/references/First Platformer Checklist.xlsx
+++ b/res/references/First Platformer Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apauley\git\platforming101\res\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E64DA0-CDC0-44F9-B7CB-81203AEA3A5E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C38ADE-C11E-4B09-8B39-2E9632023FC8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29490" yWindow="1365" windowWidth="26760" windowHeight="11790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,8 @@
     <definedName name="Ba">'Phase 2'!$B$2</definedName>
     <definedName name="Bb">'Phase 2'!$B$12</definedName>
     <definedName name="Bc">'Phase 2'!$B$22</definedName>
-    <definedName name="Bd">'Phase 2'!$B$42</definedName>
+    <definedName name="Bd">'Phase 2'!$B$32</definedName>
+    <definedName name="Be">'Phase 2'!$B$42</definedName>
     <definedName name="Ca">'Phase 3'!$B$2</definedName>
     <definedName name="Cb">'Phase 3'!$B$12</definedName>
     <definedName name="Cc">'Phase 3'!$B$22</definedName>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="72">
   <si>
     <t>Feature</t>
   </si>
@@ -561,7 +562,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="46">
+  <fills count="47">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -876,8 +877,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1100,12 +1107,21 @@
         <color indexed="64"/>
       </diagonal>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1253,9 +1269,6 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1338,20 +1351,28 @@
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1758,19 +1779,19 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="2.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" style="150" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="0.85546875" style="150" customWidth="1"/>
-    <col min="6" max="6" width="43.140625" style="151" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.85546875" style="149" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0.85546875" style="149" customWidth="1"/>
+    <col min="6" max="6" width="43.140625" style="150" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1778,20 +1799,20 @@
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="5"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="129"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="128"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="151" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="154"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="153"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1800,22 +1821,22 @@
       <c r="C3" s="124" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="130"/>
-      <c r="E3" s="130"/>
-      <c r="F3" s="131"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="130"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="122"/>
-      <c r="D4" s="132">
+      <c r="D4" s="131">
         <v>0</v>
       </c>
-      <c r="E4" s="133" t="s">
+      <c r="E4" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="134" t="s">
+      <c r="F4" s="133" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="4"/>
@@ -1824,14 +1845,14 @@
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="122"/>
-      <c r="D5" s="135">
+      <c r="D5" s="134">
         <f>D4+1</f>
         <v>1</v>
       </c>
-      <c r="E5" s="136" t="s">
+      <c r="E5" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="137" t="s">
+      <c r="F5" s="136" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="4"/>
@@ -1840,14 +1861,14 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="122"/>
-      <c r="D6" s="132">
+      <c r="D6" s="131">
         <f t="shared" ref="D6:D8" si="0">D5+1</f>
         <v>2</v>
       </c>
-      <c r="E6" s="133" t="s">
+      <c r="E6" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="134" t="s">
+      <c r="F6" s="133" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="4"/>
@@ -1856,14 +1877,14 @@
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="122"/>
-      <c r="D7" s="135">
+      <c r="D7" s="134">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E7" s="136" t="s">
+      <c r="E7" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="137" t="s">
+      <c r="F7" s="136" t="s">
         <v>62</v>
       </c>
       <c r="G7" s="4"/>
@@ -1872,14 +1893,14 @@
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="122"/>
-      <c r="D8" s="138">
+      <c r="D8" s="137">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E8" s="139" t="s">
+      <c r="E8" s="138" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="140" t="s">
+      <c r="F8" s="139" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="4"/>
@@ -1888,9 +1909,9 @@
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="128"/>
-      <c r="E9" s="128"/>
-      <c r="F9" s="129"/>
+      <c r="D9" s="127"/>
+      <c r="E9" s="127"/>
+      <c r="F9" s="128"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1899,23 +1920,23 @@
       <c r="C10" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="141"/>
-      <c r="E10" s="141"/>
-      <c r="F10" s="142"/>
+      <c r="D10" s="140"/>
+      <c r="E10" s="140"/>
+      <c r="F10" s="141"/>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="122"/>
-      <c r="D11" s="132">
+      <c r="D11" s="131">
         <f>D8+1</f>
         <v>5</v>
       </c>
-      <c r="E11" s="133" t="s">
+      <c r="E11" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="134" t="s">
+      <c r="F11" s="133" t="s">
         <v>4</v>
       </c>
       <c r="G11" s="4"/>
@@ -1924,14 +1945,14 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="122"/>
-      <c r="D12" s="135">
+      <c r="D12" s="134">
         <f t="shared" ref="D12:D15" si="1">D11+1</f>
         <v>6</v>
       </c>
-      <c r="E12" s="136" t="s">
+      <c r="E12" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="137" t="s">
+      <c r="F12" s="136" t="s">
         <v>5</v>
       </c>
       <c r="G12" s="4"/>
@@ -1940,14 +1961,14 @@
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="122"/>
-      <c r="D13" s="132">
+      <c r="D13" s="131">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="E13" s="133" t="s">
+      <c r="E13" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="134" t="s">
+      <c r="F13" s="133" t="s">
         <v>6</v>
       </c>
       <c r="G13" s="4"/>
@@ -1956,14 +1977,14 @@
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="122"/>
-      <c r="D14" s="135">
+      <c r="D14" s="134">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="E14" s="136" t="s">
+      <c r="E14" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="137" t="s">
+      <c r="F14" s="136" t="s">
         <v>69</v>
       </c>
       <c r="G14" s="4"/>
@@ -1971,15 +1992,15 @@
     <row r="15" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="126"/>
-      <c r="D15" s="132">
+      <c r="C15" s="125"/>
+      <c r="D15" s="131">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="E15" s="133" t="s">
+      <c r="E15" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="134" t="s">
+      <c r="F15" s="133" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="4"/>
@@ -1987,35 +2008,35 @@
     <row r="16" spans="1:7" ht="3.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="127"/>
-      <c r="D16" s="143"/>
-      <c r="E16" s="143"/>
-      <c r="F16" s="144"/>
+      <c r="C16" s="126"/>
+      <c r="D16" s="142"/>
+      <c r="E16" s="142"/>
+      <c r="F16" s="143"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
-      <c r="B17" s="6"/>
+      <c r="B17" s="125"/>
       <c r="C17" s="124" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="145"/>
-      <c r="E17" s="145"/>
-      <c r="F17" s="146"/>
+      <c r="D17" s="144"/>
+      <c r="E17" s="144"/>
+      <c r="F17" s="145"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="126"/>
-      <c r="D18" s="132">
+      <c r="C18" s="125"/>
+      <c r="D18" s="131">
         <f>D15+1</f>
         <v>10</v>
       </c>
-      <c r="E18" s="133" t="s">
+      <c r="E18" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="134" t="s">
+      <c r="F18" s="133" t="s">
         <v>11</v>
       </c>
       <c r="G18" s="4"/>
@@ -2023,15 +2044,15 @@
     <row r="19" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="126"/>
-      <c r="D19" s="135">
+      <c r="C19" s="125"/>
+      <c r="D19" s="134">
         <f t="shared" ref="D19:D23" si="2">D18+1</f>
         <v>11</v>
       </c>
-      <c r="E19" s="136" t="s">
+      <c r="E19" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="137" t="s">
+      <c r="F19" s="136" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="4"/>
@@ -2039,15 +2060,15 @@
     <row r="20" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="126"/>
-      <c r="D20" s="132">
+      <c r="C20" s="125"/>
+      <c r="D20" s="131">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="E20" s="133" t="s">
+      <c r="E20" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="134" t="s">
+      <c r="F20" s="133" t="s">
         <v>12</v>
       </c>
       <c r="G20" s="4"/>
@@ -2055,15 +2076,15 @@
     <row r="21" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="126"/>
-      <c r="D21" s="135">
+      <c r="C21" s="125"/>
+      <c r="D21" s="134">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="E21" s="136" t="s">
+      <c r="E21" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="F21" s="137" t="s">
+      <c r="F21" s="136" t="s">
         <v>15</v>
       </c>
       <c r="G21" s="4"/>
@@ -2071,15 +2092,15 @@
     <row r="22" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="126"/>
-      <c r="D22" s="132">
+      <c r="C22" s="125"/>
+      <c r="D22" s="131">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="E22" s="133" t="s">
+      <c r="E22" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="134" t="s">
+      <c r="F22" s="133" t="s">
         <v>16</v>
       </c>
       <c r="G22" s="4"/>
@@ -2087,15 +2108,15 @@
     <row r="23" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="138">
+      <c r="C23" s="125"/>
+      <c r="D23" s="134">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="E23" s="139" t="s">
+      <c r="E23" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="140" t="s">
+      <c r="F23" s="136" t="s">
         <v>17</v>
       </c>
       <c r="G23" s="4"/>
@@ -2103,10 +2124,10 @@
     <row r="24" spans="1:7" ht="3.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="128"/>
-      <c r="E24" s="128"/>
-      <c r="F24" s="129"/>
+      <c r="C24" s="126"/>
+      <c r="D24" s="142"/>
+      <c r="E24" s="142"/>
+      <c r="F24" s="143"/>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2115,23 +2136,23 @@
       <c r="C25" s="123" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="141"/>
-      <c r="E25" s="141"/>
-      <c r="F25" s="142"/>
+      <c r="D25" s="140"/>
+      <c r="E25" s="140"/>
+      <c r="F25" s="141"/>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="132">
+      <c r="C26" s="167"/>
+      <c r="D26" s="131">
         <f>D23+1</f>
         <v>16</v>
       </c>
-      <c r="E26" s="133" t="s">
+      <c r="E26" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="134" t="s">
+      <c r="F26" s="164" t="s">
         <v>19</v>
       </c>
       <c r="G26" s="4"/>
@@ -2140,14 +2161,14 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="135">
+      <c r="D27" s="134">
         <f t="shared" ref="D27:D34" si="3">D26+1</f>
         <v>17</v>
       </c>
-      <c r="E27" s="136" t="s">
+      <c r="E27" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="137" t="s">
+      <c r="F27" s="136" t="s">
         <v>20</v>
       </c>
       <c r="G27" s="4"/>
@@ -2156,14 +2177,14 @@
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="132">
+      <c r="D28" s="131">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="E28" s="133" t="s">
+      <c r="E28" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="134" t="s">
+      <c r="F28" s="133" t="s">
         <v>21</v>
       </c>
       <c r="G28" s="4"/>
@@ -2172,14 +2193,14 @@
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="135">
+      <c r="D29" s="134">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="E29" s="136" t="s">
+      <c r="E29" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="137" t="s">
+      <c r="F29" s="136" t="s">
         <v>22</v>
       </c>
       <c r="G29" s="4"/>
@@ -2188,14 +2209,14 @@
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="132">
+      <c r="D30" s="131">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="E30" s="133" t="s">
+      <c r="E30" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="134" t="s">
+      <c r="F30" s="133" t="s">
         <v>23</v>
       </c>
       <c r="G30" s="4"/>
@@ -2204,14 +2225,14 @@
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="135">
+      <c r="D31" s="134">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="E31" s="136" t="s">
+      <c r="E31" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="137" t="s">
+      <c r="F31" s="136" t="s">
         <v>24</v>
       </c>
       <c r="G31" s="4"/>
@@ -2220,14 +2241,14 @@
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="7"/>
-      <c r="D32" s="132">
+      <c r="D32" s="131">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="E32" s="133" t="s">
+      <c r="E32" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="134" t="s">
+      <c r="F32" s="133" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="4"/>
@@ -2236,14 +2257,14 @@
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="132">
+      <c r="D33" s="134">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="E33" s="133" t="s">
+      <c r="E33" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="F33" s="134" t="s">
+      <c r="F33" s="136" t="s">
         <v>26</v>
       </c>
       <c r="G33" s="4"/>
@@ -2252,14 +2273,14 @@
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="147">
+      <c r="D34" s="131">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="E34" s="148" t="s">
+      <c r="E34" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F34" s="149" t="s">
+      <c r="F34" s="133" t="s">
         <v>48</v>
       </c>
       <c r="G34" s="4"/>
@@ -2267,10 +2288,10 @@
     <row r="35" spans="1:7" ht="3.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
-      <c r="C35" s="125"/>
-      <c r="D35" s="128"/>
-      <c r="E35" s="128"/>
-      <c r="F35" s="129"/>
+      <c r="C35" s="126"/>
+      <c r="D35" s="142"/>
+      <c r="E35" s="142"/>
+      <c r="F35" s="143"/>
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2279,23 +2300,23 @@
       <c r="C36" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="145"/>
-      <c r="E36" s="145"/>
-      <c r="F36" s="146"/>
+      <c r="D36" s="144"/>
+      <c r="E36" s="144"/>
+      <c r="F36" s="145"/>
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="132">
+      <c r="D37" s="131">
         <f>D34+1</f>
         <v>25</v>
       </c>
-      <c r="E37" s="133" t="s">
+      <c r="E37" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F37" s="134" t="s">
+      <c r="F37" s="133" t="s">
         <v>28</v>
       </c>
       <c r="G37" s="4"/>
@@ -2304,14 +2325,14 @@
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="7"/>
-      <c r="D38" s="135">
+      <c r="D38" s="134">
         <f t="shared" ref="D38:D46" si="4">D37+1</f>
         <v>26</v>
       </c>
-      <c r="E38" s="136" t="s">
+      <c r="E38" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="F38" s="137" t="s">
+      <c r="F38" s="136" t="s">
         <v>29</v>
       </c>
       <c r="G38" s="4"/>
@@ -2320,14 +2341,14 @@
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="7"/>
-      <c r="D39" s="132">
+      <c r="D39" s="131">
         <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="E39" s="133" t="s">
+      <c r="E39" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F39" s="134" t="s">
+      <c r="F39" s="133" t="s">
         <v>30</v>
       </c>
       <c r="G39" s="4"/>
@@ -2336,14 +2357,14 @@
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="7"/>
-      <c r="D40" s="135">
+      <c r="D40" s="134">
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="E40" s="136" t="s">
+      <c r="E40" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="F40" s="137" t="s">
+      <c r="F40" s="136" t="s">
         <v>31</v>
       </c>
       <c r="G40" s="4"/>
@@ -2352,14 +2373,14 @@
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="7"/>
-      <c r="D41" s="132">
+      <c r="D41" s="131">
         <f t="shared" si="4"/>
         <v>29</v>
       </c>
-      <c r="E41" s="133" t="s">
+      <c r="E41" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F41" s="134" t="s">
+      <c r="F41" s="133" t="s">
         <v>32</v>
       </c>
       <c r="G41" s="4"/>
@@ -2368,14 +2389,14 @@
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="7"/>
-      <c r="D42" s="135">
+      <c r="D42" s="134">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="E42" s="136" t="s">
+      <c r="E42" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="F42" s="137" t="s">
+      <c r="F42" s="136" t="s">
         <v>33</v>
       </c>
       <c r="G42" s="4"/>
@@ -2384,14 +2405,14 @@
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="7"/>
-      <c r="D43" s="132">
+      <c r="D43" s="131">
         <f t="shared" si="4"/>
         <v>31</v>
       </c>
-      <c r="E43" s="133" t="s">
+      <c r="E43" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F43" s="134" t="s">
+      <c r="F43" s="133" t="s">
         <v>63</v>
       </c>
       <c r="G43" s="4"/>
@@ -2400,14 +2421,14 @@
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="7"/>
-      <c r="D44" s="135">
+      <c r="D44" s="134">
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
-      <c r="E44" s="136" t="s">
+      <c r="E44" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="F44" s="137" t="s">
+      <c r="F44" s="136" t="s">
         <v>34</v>
       </c>
       <c r="G44" s="4"/>
@@ -2416,30 +2437,42 @@
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="7"/>
-      <c r="D45" s="132">
+      <c r="D45" s="131">
         <f t="shared" si="4"/>
         <v>33</v>
       </c>
-      <c r="E45" s="133" t="s">
+      <c r="E45" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="F45" s="134" t="s">
+      <c r="F45" s="133" t="s">
         <v>70</v>
       </c>
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
       <c r="C46" s="7"/>
-      <c r="D46" s="147">
+      <c r="D46" s="146">
         <f t="shared" si="4"/>
         <v>34</v>
       </c>
-      <c r="E46" s="148" t="s">
+      <c r="E46" s="147" t="s">
         <v>35</v>
       </c>
-      <c r="F46" s="149" t="s">
+      <c r="F46" s="148" t="s">
         <v>71</v>
       </c>
+      <c r="G46" s="4"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="165"/>
+      <c r="E47" s="165"/>
+      <c r="F47" s="166"/>
+      <c r="G47" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2481,11 +2514,19 @@
     <hyperlink ref="D43:F43" location="Eg" display="g" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
     <hyperlink ref="D44:F44" location="Eh" display="h" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
     <hyperlink ref="F4" location="Aa" display="Player spawns on screen" xr:uid="{737FFEE2-DFD5-42C6-B858-2FCEF8EC9F7D}"/>
-    <hyperlink ref="D18" location="Ba" display="a" xr:uid="{398B4FB7-3A48-473F-98F0-BC34A0A83F75}"/>
-    <hyperlink ref="D26" location="Ba" display="a" xr:uid="{EFDB2CFE-CC8D-43E9-8E35-81704B9DD70E}"/>
+    <hyperlink ref="D18" location="Ca" display="Ca" xr:uid="{398B4FB7-3A48-473F-98F0-BC34A0A83F75}"/>
+    <hyperlink ref="D26" location="Da" display="Da" xr:uid="{EFDB2CFE-CC8D-43E9-8E35-81704B9DD70E}"/>
     <hyperlink ref="D37" location="Ba" display="a" xr:uid="{93F0514F-0A15-4AA2-AE5C-F68C4F8FB0BE}"/>
     <hyperlink ref="D45:F45" location="Eg" display="g" xr:uid="{4972F980-79FD-4AE3-92A1-794E254C95D3}"/>
     <hyperlink ref="D46:F46" location="Eh" display="h" xr:uid="{FBFDCAC7-88B0-4B95-B4C4-2A42E51FD61D}"/>
+    <hyperlink ref="F18" location="Ca" display="Enemies spawn" xr:uid="{3E7BE159-F50D-42FD-ACF3-7450FB970965}"/>
+    <hyperlink ref="D4" location="Aa" display="Aa" xr:uid="{78C876B7-C0F0-4746-A906-DC11CE02D2EA}"/>
+    <hyperlink ref="D14" location="Bd" display="Bd" xr:uid="{3D8DFBD4-D059-4889-8D7E-5E3C32ADA276}"/>
+    <hyperlink ref="D15" location="Be" display="Be" xr:uid="{F74FCEF7-3AB5-4602-B906-2687C0E39066}"/>
+    <hyperlink ref="F14" location="Bd" display="Player can run" xr:uid="{E842AF3A-2744-4A46-AD1C-6EC6B402135F}"/>
+    <hyperlink ref="F15" location="Be" display="Camera will follow player" xr:uid="{82CF404E-DB41-4910-8FEF-4E3E22B0CF8C}"/>
+    <hyperlink ref="F26" location="Da" display="Bullets tracked" xr:uid="{3EA2439B-148E-4FC6-92B8-85C7BD338919}"/>
+    <hyperlink ref="E18" location="Ca" display="-" xr:uid="{75713649-6603-42CD-A60D-C7FBC48394F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2499,7 +2540,7 @@
   </sheetPr>
   <dimension ref="B2:P50"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -3111,7 +3152,7 @@
   </sheetPr>
   <dimension ref="B2:O50"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -3732,12 +3773,12 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4">
-    <tabColor rgb="FFFFE38B"/>
+    <tabColor theme="0" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="B2:O60"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="AB48" sqref="AB48"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4456,8 +4497,8 @@
   </sheetPr>
   <dimension ref="B2:X96"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4999,12 +5040,12 @@
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="69"/>
       <c r="C45" s="76"/>
-      <c r="D45" s="155" t="s">
+      <c r="D45" s="154" t="s">
         <v>41</v>
       </c>
-      <c r="E45" s="155"/>
-      <c r="F45" s="155"/>
-      <c r="G45" s="155"/>
+      <c r="E45" s="154"/>
+      <c r="F45" s="154"/>
+      <c r="G45" s="154"/>
       <c r="H45" s="76"/>
       <c r="I45" s="55"/>
       <c r="O45" s="11"/>
@@ -5012,12 +5053,12 @@
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="69"/>
       <c r="C46" s="76"/>
-      <c r="D46" s="156" t="s">
+      <c r="D46" s="155" t="s">
         <v>42</v>
       </c>
-      <c r="E46" s="157"/>
-      <c r="F46" s="157"/>
-      <c r="G46" s="157"/>
+      <c r="E46" s="156"/>
+      <c r="F46" s="156"/>
+      <c r="G46" s="156"/>
       <c r="H46" s="76"/>
       <c r="I46" s="55"/>
       <c r="O46" s="11"/>
@@ -5025,12 +5066,12 @@
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="69"/>
       <c r="C47" s="76"/>
-      <c r="D47" s="159" t="s">
+      <c r="D47" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="E47" s="159"/>
-      <c r="F47" s="159"/>
-      <c r="G47" s="159"/>
+      <c r="E47" s="158"/>
+      <c r="F47" s="158"/>
+      <c r="G47" s="158"/>
       <c r="H47" s="76"/>
       <c r="I47" s="55"/>
       <c r="N47" s="60"/>
@@ -5039,12 +5080,12 @@
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="69"/>
       <c r="C48" s="76"/>
-      <c r="D48" s="156" t="s">
+      <c r="D48" s="155" t="s">
         <v>43</v>
       </c>
-      <c r="E48" s="156"/>
-      <c r="F48" s="156"/>
-      <c r="G48" s="156"/>
+      <c r="E48" s="155"/>
+      <c r="F48" s="155"/>
+      <c r="G48" s="155"/>
       <c r="H48" s="76"/>
       <c r="I48" s="74"/>
       <c r="J48" s="11"/>
@@ -5249,26 +5290,26 @@
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B65" s="69"/>
-      <c r="C65" s="158" t="s">
+      <c r="C65" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="D65" s="158"/>
-      <c r="E65" s="158"/>
-      <c r="F65" s="158"/>
-      <c r="G65" s="158"/>
-      <c r="H65" s="158"/>
+      <c r="D65" s="157"/>
+      <c r="E65" s="157"/>
+      <c r="F65" s="157"/>
+      <c r="G65" s="157"/>
+      <c r="H65" s="157"/>
       <c r="I65" s="55"/>
       <c r="O65" s="11"/>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="69"/>
       <c r="C66" s="76"/>
-      <c r="D66" s="155" t="s">
+      <c r="D66" s="154" t="s">
         <v>45</v>
       </c>
-      <c r="E66" s="155"/>
-      <c r="F66" s="155"/>
-      <c r="G66" s="155"/>
+      <c r="E66" s="154"/>
+      <c r="F66" s="154"/>
+      <c r="G66" s="154"/>
       <c r="H66" s="76"/>
       <c r="I66" s="55"/>
       <c r="O66" s="11"/>
@@ -5276,12 +5317,12 @@
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B67" s="69"/>
       <c r="C67" s="76"/>
-      <c r="D67" s="156" t="s">
+      <c r="D67" s="155" t="s">
         <v>46</v>
       </c>
-      <c r="E67" s="157"/>
-      <c r="F67" s="157"/>
-      <c r="G67" s="157"/>
+      <c r="E67" s="156"/>
+      <c r="F67" s="156"/>
+      <c r="G67" s="156"/>
       <c r="H67" s="76"/>
       <c r="I67" s="55"/>
       <c r="N67" s="28"/>
@@ -5290,12 +5331,12 @@
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B68" s="69"/>
       <c r="C68" s="76"/>
-      <c r="D68" s="156" t="s">
+      <c r="D68" s="155" t="s">
         <v>43</v>
       </c>
-      <c r="E68" s="156"/>
-      <c r="F68" s="156"/>
-      <c r="G68" s="156"/>
+      <c r="E68" s="155"/>
+      <c r="F68" s="155"/>
+      <c r="G68" s="155"/>
       <c r="H68" s="76"/>
       <c r="I68" s="55"/>
       <c r="J68" s="11"/>
@@ -6374,12 +6415,12 @@
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="32"/>
       <c r="C44" s="76"/>
-      <c r="D44" s="160" t="s">
+      <c r="D44" s="163" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="160"/>
-      <c r="F44" s="160"/>
-      <c r="G44" s="160"/>
+      <c r="E44" s="163"/>
+      <c r="F44" s="163"/>
+      <c r="G44" s="163"/>
       <c r="H44" s="76"/>
       <c r="I44" s="34"/>
     </row>
@@ -6401,50 +6442,50 @@
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="32"/>
-      <c r="C46" s="162" t="s">
+      <c r="C46" s="159" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="162"/>
+      <c r="D46" s="159"/>
       <c r="E46" s="121" t="s">
         <v>54</v>
       </c>
-      <c r="F46" s="162">
+      <c r="F46" s="159">
         <v>8999</v>
       </c>
-      <c r="G46" s="162"/>
-      <c r="H46" s="162"/>
+      <c r="G46" s="159"/>
+      <c r="H46" s="159"/>
       <c r="I46" s="34"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="32"/>
-      <c r="C47" s="162" t="s">
+      <c r="C47" s="159" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="162"/>
+      <c r="D47" s="159"/>
       <c r="E47" s="121" t="s">
         <v>54</v>
       </c>
-      <c r="F47" s="162">
+      <c r="F47" s="159">
         <v>1337</v>
       </c>
-      <c r="G47" s="162"/>
-      <c r="H47" s="162"/>
+      <c r="G47" s="159"/>
+      <c r="H47" s="159"/>
       <c r="I47" s="34"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="32"/>
-      <c r="C48" s="162" t="s">
+      <c r="C48" s="159" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="162"/>
+      <c r="D48" s="159"/>
       <c r="E48" s="121" t="s">
         <v>54</v>
       </c>
-      <c r="F48" s="162">
+      <c r="F48" s="159">
         <v>-5</v>
       </c>
-      <c r="G48" s="162"/>
-      <c r="H48" s="162"/>
+      <c r="G48" s="159"/>
+      <c r="H48" s="159"/>
       <c r="I48" s="34"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
@@ -6514,12 +6555,12 @@
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="89"/>
       <c r="C55" s="76"/>
-      <c r="D55" s="155" t="s">
+      <c r="D55" s="154" t="s">
         <v>41</v>
       </c>
-      <c r="E55" s="155"/>
-      <c r="F55" s="155"/>
-      <c r="G55" s="155"/>
+      <c r="E55" s="154"/>
+      <c r="F55" s="154"/>
+      <c r="G55" s="154"/>
       <c r="H55" s="76"/>
       <c r="I55" s="81"/>
       <c r="J55" s="82"/>
@@ -6532,12 +6573,12 @@
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" s="89"/>
       <c r="C56" s="76"/>
-      <c r="D56" s="156" t="s">
+      <c r="D56" s="155" t="s">
         <v>42</v>
       </c>
-      <c r="E56" s="157"/>
-      <c r="F56" s="157"/>
-      <c r="G56" s="157"/>
+      <c r="E56" s="156"/>
+      <c r="F56" s="156"/>
+      <c r="G56" s="156"/>
       <c r="H56" s="76"/>
       <c r="I56" s="81"/>
       <c r="J56" s="82"/>
@@ -6550,12 +6591,12 @@
     <row r="57" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="89"/>
       <c r="C57" s="76"/>
-      <c r="D57" s="156" t="s">
+      <c r="D57" s="155" t="s">
         <v>44</v>
       </c>
-      <c r="E57" s="157"/>
-      <c r="F57" s="157"/>
-      <c r="G57" s="157"/>
+      <c r="E57" s="156"/>
+      <c r="F57" s="156"/>
+      <c r="G57" s="156"/>
       <c r="H57" s="76"/>
       <c r="I57" s="81"/>
       <c r="J57" s="82"/>
@@ -6568,12 +6609,12 @@
     <row r="58" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="89"/>
       <c r="C58" s="76"/>
-      <c r="D58" s="159" t="s">
+      <c r="D58" s="158" t="s">
         <v>60</v>
       </c>
-      <c r="E58" s="159"/>
-      <c r="F58" s="159"/>
-      <c r="G58" s="159"/>
+      <c r="E58" s="158"/>
+      <c r="F58" s="158"/>
+      <c r="G58" s="158"/>
       <c r="H58" s="76"/>
       <c r="I58" s="88"/>
       <c r="J58" s="86"/>
@@ -6643,14 +6684,14 @@
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B64" s="32"/>
-      <c r="C64" s="155" t="s">
+      <c r="C64" s="154" t="s">
         <v>64</v>
       </c>
-      <c r="D64" s="155"/>
-      <c r="E64" s="155"/>
-      <c r="F64" s="155"/>
-      <c r="G64" s="155"/>
-      <c r="H64" s="155"/>
+      <c r="D64" s="154"/>
+      <c r="E64" s="154"/>
+      <c r="F64" s="154"/>
+      <c r="G64" s="154"/>
+      <c r="H64" s="154"/>
       <c r="I64" s="34"/>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
@@ -6665,18 +6706,18 @@
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="32"/>
-      <c r="C66" s="162" t="s">
+      <c r="C66" s="159" t="s">
         <v>65</v>
       </c>
-      <c r="D66" s="162"/>
+      <c r="D66" s="159"/>
       <c r="E66" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="F66" s="163" t="s">
+      <c r="F66" s="160" t="s">
         <v>66</v>
       </c>
-      <c r="G66" s="163"/>
-      <c r="H66" s="163"/>
+      <c r="G66" s="160"/>
+      <c r="H66" s="160"/>
       <c r="I66" s="34"/>
     </row>
     <row r="67" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6688,27 +6729,27 @@
       <c r="E67" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="F67" s="164" t="s">
+      <c r="F67" s="162" t="s">
         <v>66</v>
       </c>
-      <c r="G67" s="164"/>
-      <c r="H67" s="164"/>
+      <c r="G67" s="162"/>
+      <c r="H67" s="162"/>
       <c r="I67" s="34"/>
     </row>
     <row r="68" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="32"/>
-      <c r="C68" s="162" t="s">
+      <c r="C68" s="159" t="s">
         <v>67</v>
       </c>
-      <c r="D68" s="162"/>
+      <c r="D68" s="159"/>
       <c r="E68" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="F68" s="163" t="s">
+      <c r="F68" s="160" t="s">
         <v>66</v>
       </c>
-      <c r="G68" s="163"/>
-      <c r="H68" s="163"/>
+      <c r="G68" s="160"/>
+      <c r="H68" s="160"/>
       <c r="I68" s="34"/>
     </row>
     <row r="69" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7545,13 +7586,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="C64:H64"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="F67:H67"/>
     <mergeCell ref="D44:G44"/>
     <mergeCell ref="D57:G57"/>
     <mergeCell ref="D58:G58"/>
@@ -7565,6 +7599,13 @@
     <mergeCell ref="F47:H47"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="F48:H48"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="C64:H64"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="F67:H67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
20191126 - Enemy Health Tracking
</commit_message>
<xml_diff>
--- a/res/references/First Platformer Checklist.xlsx
+++ b/res/references/First Platformer Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apauley\git\platforming101\res\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD603504-21C4-4EF9-97C0-900867E5E88E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91B91CD-87E5-4339-8C4C-D12A914474A0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="1830" windowWidth="26760" windowHeight="11790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="26760" windowHeight="11790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="81">
   <si>
     <t>Feature</t>
   </si>
@@ -361,6 +361,21 @@
   </si>
   <si>
     <t>+ Animations</t>
+  </si>
+  <si>
+    <t>+ Sound Effects</t>
+  </si>
+  <si>
+    <t>+ Music</t>
+  </si>
+  <si>
+    <t>+ Audio Manipulation</t>
+  </si>
+  <si>
+    <t>+Loadout Select</t>
+  </si>
+  <si>
+    <t>+Unlocks</t>
   </si>
 </sst>
 </file>
@@ -1330,6 +1345,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1354,26 +1374,21 @@
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1781,8 +1796,8 @@
   </sheetPr>
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1806,13 +1821,13 @@
     </row>
     <row r="2" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="149" t="s">
+      <c r="B2" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="151"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="154"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2176,7 +2191,7 @@
     <row r="28" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="162"/>
+      <c r="C28" s="149"/>
       <c r="D28" s="130">
         <f>D27+1</f>
         <v>18</v>
@@ -2220,7 +2235,7 @@
         <v>21</v>
       </c>
       <c r="G30" s="4"/>
-      <c r="H30" s="164" t="s">
+      <c r="H30" s="151" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2239,6 +2254,9 @@
         <v>22</v>
       </c>
       <c r="G31" s="4"/>
+      <c r="H31" s="151" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
@@ -2255,8 +2273,11 @@
         <v>23</v>
       </c>
       <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H32" s="151" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="7"/>
@@ -2272,7 +2293,7 @@
       </c>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="7"/>
@@ -2288,7 +2309,7 @@
       </c>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="7"/>
@@ -2304,7 +2325,7 @@
       </c>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="7"/>
@@ -2320,7 +2341,7 @@
       </c>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" ht="3.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="3.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="125"/>
@@ -2329,7 +2350,7 @@
       <c r="F37" s="142"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="6"/>
       <c r="C38" s="123" t="s">
@@ -2340,7 +2361,7 @@
       <c r="F38" s="144"/>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="7"/>
@@ -2356,12 +2377,12 @@
       </c>
       <c r="G39" s="4"/>
     </row>
-    <row r="40" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="7"/>
       <c r="D40" s="133">
-        <f>D39+1</f>
+        <f t="shared" ref="D40:D47" si="4">D39+1</f>
         <v>28</v>
       </c>
       <c r="E40" s="134" t="s">
@@ -2372,12 +2393,12 @@
       </c>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="7"/>
       <c r="D41" s="130">
-        <f>D40+1</f>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="E41" s="131" t="s">
@@ -2388,12 +2409,12 @@
       </c>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="7"/>
       <c r="D42" s="133">
-        <f>D41+1</f>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="E42" s="134" t="s">
@@ -2404,12 +2425,12 @@
       </c>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="7"/>
       <c r="D43" s="130">
-        <f>D42+1</f>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="E43" s="131" t="s">
@@ -2420,12 +2441,12 @@
       </c>
       <c r="G43" s="4"/>
     </row>
-    <row r="44" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="7"/>
       <c r="D44" s="133">
-        <f>D43+1</f>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="E44" s="134" t="s">
@@ -2435,13 +2456,16 @@
         <v>33</v>
       </c>
       <c r="G44" s="4"/>
-    </row>
-    <row r="45" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H44" s="151" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="7"/>
       <c r="D45" s="130">
-        <f>D44+1</f>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="E45" s="131" t="s">
@@ -2451,13 +2475,16 @@
         <v>63</v>
       </c>
       <c r="G45" s="4"/>
-    </row>
-    <row r="46" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H45" s="151" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="7"/>
       <c r="D46" s="133">
-        <f>D45+1</f>
+        <f t="shared" si="4"/>
         <v>34</v>
       </c>
       <c r="E46" s="134" t="s">
@@ -2467,13 +2494,16 @@
         <v>34</v>
       </c>
       <c r="G46" s="4"/>
-    </row>
-    <row r="47" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H46" s="151" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="7"/>
       <c r="D47" s="130">
-        <f>D46+1</f>
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
       <c r="E47" s="131" t="s">
@@ -2484,7 +2514,7 @@
       </c>
       <c r="G47" s="4"/>
     </row>
-    <row r="48" spans="1:7" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="7"/>
@@ -4852,8 +4882,8 @@
       <c r="G26" s="13"/>
       <c r="H26" s="41"/>
       <c r="I26" s="42"/>
-      <c r="K26" s="163"/>
-      <c r="N26" s="163"/>
+      <c r="K26" s="150"/>
+      <c r="N26" s="150"/>
       <c r="O26" s="10"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
@@ -5329,12 +5359,12 @@
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B65" s="68"/>
       <c r="C65" s="75"/>
-      <c r="D65" s="152" t="s">
+      <c r="D65" s="155" t="s">
         <v>41</v>
       </c>
-      <c r="E65" s="152"/>
-      <c r="F65" s="152"/>
-      <c r="G65" s="152"/>
+      <c r="E65" s="155"/>
+      <c r="F65" s="155"/>
+      <c r="G65" s="155"/>
       <c r="H65" s="75"/>
       <c r="I65" s="54"/>
       <c r="O65" s="10"/>
@@ -5342,12 +5372,12 @@
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="68"/>
       <c r="C66" s="75"/>
-      <c r="D66" s="153" t="s">
+      <c r="D66" s="156" t="s">
         <v>42</v>
       </c>
-      <c r="E66" s="154"/>
-      <c r="F66" s="154"/>
-      <c r="G66" s="154"/>
+      <c r="E66" s="157"/>
+      <c r="F66" s="157"/>
+      <c r="G66" s="157"/>
       <c r="H66" s="75"/>
       <c r="I66" s="54"/>
       <c r="O66" s="10"/>
@@ -5355,12 +5385,12 @@
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B67" s="68"/>
       <c r="C67" s="75"/>
-      <c r="D67" s="156" t="s">
+      <c r="D67" s="159" t="s">
         <v>44</v>
       </c>
-      <c r="E67" s="156"/>
-      <c r="F67" s="156"/>
-      <c r="G67" s="156"/>
+      <c r="E67" s="159"/>
+      <c r="F67" s="159"/>
+      <c r="G67" s="159"/>
       <c r="H67" s="75"/>
       <c r="I67" s="54"/>
       <c r="N67" s="59"/>
@@ -5369,12 +5399,12 @@
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B68" s="68"/>
       <c r="C68" s="75"/>
-      <c r="D68" s="153" t="s">
+      <c r="D68" s="156" t="s">
         <v>43</v>
       </c>
-      <c r="E68" s="153"/>
-      <c r="F68" s="153"/>
-      <c r="G68" s="153"/>
+      <c r="E68" s="156"/>
+      <c r="F68" s="156"/>
+      <c r="G68" s="156"/>
       <c r="H68" s="75"/>
       <c r="I68" s="73"/>
       <c r="J68" s="10"/>
@@ -5579,26 +5609,26 @@
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B85" s="68"/>
-      <c r="C85" s="155" t="s">
+      <c r="C85" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="D85" s="155"/>
-      <c r="E85" s="155"/>
-      <c r="F85" s="155"/>
-      <c r="G85" s="155"/>
-      <c r="H85" s="155"/>
+      <c r="D85" s="158"/>
+      <c r="E85" s="158"/>
+      <c r="F85" s="158"/>
+      <c r="G85" s="158"/>
+      <c r="H85" s="158"/>
       <c r="I85" s="54"/>
       <c r="O85" s="10"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B86" s="68"/>
       <c r="C86" s="75"/>
-      <c r="D86" s="152" t="s">
+      <c r="D86" s="155" t="s">
         <v>45</v>
       </c>
-      <c r="E86" s="152"/>
-      <c r="F86" s="152"/>
-      <c r="G86" s="152"/>
+      <c r="E86" s="155"/>
+      <c r="F86" s="155"/>
+      <c r="G86" s="155"/>
       <c r="H86" s="75"/>
       <c r="I86" s="54"/>
       <c r="O86" s="10"/>
@@ -5606,12 +5636,12 @@
     <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B87" s="68"/>
       <c r="C87" s="75"/>
-      <c r="D87" s="153" t="s">
+      <c r="D87" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="E87" s="154"/>
-      <c r="F87" s="154"/>
-      <c r="G87" s="154"/>
+      <c r="E87" s="157"/>
+      <c r="F87" s="157"/>
+      <c r="G87" s="157"/>
       <c r="H87" s="75"/>
       <c r="I87" s="54"/>
       <c r="N87" s="27"/>
@@ -5620,12 +5650,12 @@
     <row r="88" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B88" s="68"/>
       <c r="C88" s="75"/>
-      <c r="D88" s="153" t="s">
+      <c r="D88" s="156" t="s">
         <v>43</v>
       </c>
-      <c r="E88" s="153"/>
-      <c r="F88" s="153"/>
-      <c r="G88" s="153"/>
+      <c r="E88" s="156"/>
+      <c r="F88" s="156"/>
+      <c r="G88" s="156"/>
       <c r="H88" s="75"/>
       <c r="I88" s="54"/>
       <c r="J88" s="10"/>
@@ -6704,77 +6734,77 @@
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="31"/>
       <c r="C44" s="75"/>
-      <c r="D44" s="157" t="s">
+      <c r="D44" s="164" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="157"/>
-      <c r="F44" s="157"/>
-      <c r="G44" s="157"/>
+      <c r="E44" s="164"/>
+      <c r="F44" s="164"/>
+      <c r="G44" s="164"/>
       <c r="H44" s="75"/>
       <c r="I44" s="33"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="31"/>
-      <c r="C45" s="158" t="s">
+      <c r="C45" s="162" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="158"/>
+      <c r="D45" s="162"/>
       <c r="E45" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="F45" s="158">
+      <c r="F45" s="162">
         <v>9001</v>
       </c>
-      <c r="G45" s="158"/>
-      <c r="H45" s="158"/>
+      <c r="G45" s="162"/>
+      <c r="H45" s="162"/>
       <c r="I45" s="33"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="31"/>
-      <c r="C46" s="159" t="s">
+      <c r="C46" s="160" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="159"/>
+      <c r="D46" s="160"/>
       <c r="E46" s="120" t="s">
         <v>54</v>
       </c>
-      <c r="F46" s="159">
+      <c r="F46" s="160">
         <v>8999</v>
       </c>
-      <c r="G46" s="159"/>
-      <c r="H46" s="159"/>
+      <c r="G46" s="160"/>
+      <c r="H46" s="160"/>
       <c r="I46" s="33"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="31"/>
-      <c r="C47" s="159" t="s">
+      <c r="C47" s="160" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="159"/>
+      <c r="D47" s="160"/>
       <c r="E47" s="120" t="s">
         <v>54</v>
       </c>
-      <c r="F47" s="159">
+      <c r="F47" s="160">
         <v>1337</v>
       </c>
-      <c r="G47" s="159"/>
-      <c r="H47" s="159"/>
+      <c r="G47" s="160"/>
+      <c r="H47" s="160"/>
       <c r="I47" s="33"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="31"/>
-      <c r="C48" s="159" t="s">
+      <c r="C48" s="160" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="159"/>
+      <c r="D48" s="160"/>
       <c r="E48" s="120" t="s">
         <v>54</v>
       </c>
-      <c r="F48" s="159">
+      <c r="F48" s="160">
         <v>-5</v>
       </c>
-      <c r="G48" s="159"/>
-      <c r="H48" s="159"/>
+      <c r="G48" s="160"/>
+      <c r="H48" s="160"/>
       <c r="I48" s="33"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
@@ -6844,12 +6874,12 @@
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="88"/>
       <c r="C55" s="75"/>
-      <c r="D55" s="152" t="s">
+      <c r="D55" s="155" t="s">
         <v>41</v>
       </c>
-      <c r="E55" s="152"/>
-      <c r="F55" s="152"/>
-      <c r="G55" s="152"/>
+      <c r="E55" s="155"/>
+      <c r="F55" s="155"/>
+      <c r="G55" s="155"/>
       <c r="H55" s="75"/>
       <c r="I55" s="80"/>
       <c r="J55" s="81"/>
@@ -6862,12 +6892,12 @@
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" s="88"/>
       <c r="C56" s="75"/>
-      <c r="D56" s="153" t="s">
+      <c r="D56" s="156" t="s">
         <v>42</v>
       </c>
-      <c r="E56" s="154"/>
-      <c r="F56" s="154"/>
-      <c r="G56" s="154"/>
+      <c r="E56" s="157"/>
+      <c r="F56" s="157"/>
+      <c r="G56" s="157"/>
       <c r="H56" s="75"/>
       <c r="I56" s="80"/>
       <c r="J56" s="81"/>
@@ -6880,12 +6910,12 @@
     <row r="57" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="88"/>
       <c r="C57" s="75"/>
-      <c r="D57" s="153" t="s">
+      <c r="D57" s="156" t="s">
         <v>44</v>
       </c>
-      <c r="E57" s="154"/>
-      <c r="F57" s="154"/>
-      <c r="G57" s="154"/>
+      <c r="E57" s="157"/>
+      <c r="F57" s="157"/>
+      <c r="G57" s="157"/>
       <c r="H57" s="75"/>
       <c r="I57" s="80"/>
       <c r="J57" s="81"/>
@@ -6898,12 +6928,12 @@
     <row r="58" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="88"/>
       <c r="C58" s="75"/>
-      <c r="D58" s="156" t="s">
+      <c r="D58" s="159" t="s">
         <v>60</v>
       </c>
-      <c r="E58" s="156"/>
-      <c r="F58" s="156"/>
-      <c r="G58" s="156"/>
+      <c r="E58" s="159"/>
+      <c r="F58" s="159"/>
+      <c r="G58" s="159"/>
       <c r="H58" s="75"/>
       <c r="I58" s="87"/>
       <c r="J58" s="85"/>
@@ -6973,14 +7003,14 @@
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B64" s="31"/>
-      <c r="C64" s="152" t="s">
+      <c r="C64" s="155" t="s">
         <v>64</v>
       </c>
-      <c r="D64" s="152"/>
-      <c r="E64" s="152"/>
-      <c r="F64" s="152"/>
-      <c r="G64" s="152"/>
-      <c r="H64" s="152"/>
+      <c r="D64" s="155"/>
+      <c r="E64" s="155"/>
+      <c r="F64" s="155"/>
+      <c r="G64" s="155"/>
+      <c r="H64" s="155"/>
       <c r="I64" s="33"/>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
@@ -6995,50 +7025,50 @@
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="31"/>
-      <c r="C66" s="159" t="s">
+      <c r="C66" s="160" t="s">
         <v>65</v>
       </c>
-      <c r="D66" s="159"/>
+      <c r="D66" s="160"/>
       <c r="E66" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="F66" s="160" t="s">
+      <c r="F66" s="161" t="s">
         <v>66</v>
       </c>
-      <c r="G66" s="160"/>
-      <c r="H66" s="160"/>
+      <c r="G66" s="161"/>
+      <c r="H66" s="161"/>
       <c r="I66" s="33"/>
     </row>
     <row r="67" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="31"/>
-      <c r="C67" s="158" t="s">
+      <c r="C67" s="162" t="s">
         <v>68</v>
       </c>
-      <c r="D67" s="158"/>
+      <c r="D67" s="162"/>
       <c r="E67" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="F67" s="161" t="s">
+      <c r="F67" s="163" t="s">
         <v>66</v>
       </c>
-      <c r="G67" s="161"/>
-      <c r="H67" s="161"/>
+      <c r="G67" s="163"/>
+      <c r="H67" s="163"/>
       <c r="I67" s="33"/>
     </row>
     <row r="68" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="31"/>
-      <c r="C68" s="159" t="s">
+      <c r="C68" s="160" t="s">
         <v>67</v>
       </c>
-      <c r="D68" s="159"/>
+      <c r="D68" s="160"/>
       <c r="E68" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="F68" s="160" t="s">
+      <c r="F68" s="161" t="s">
         <v>66</v>
       </c>
-      <c r="G68" s="160"/>
-      <c r="H68" s="160"/>
+      <c r="G68" s="161"/>
+      <c r="H68" s="161"/>
       <c r="I68" s="33"/>
     </row>
     <row r="69" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7875,13 +7905,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="C64:H64"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="F67:H67"/>
     <mergeCell ref="D44:G44"/>
     <mergeCell ref="D57:G57"/>
     <mergeCell ref="D58:G58"/>
@@ -7895,6 +7918,13 @@
     <mergeCell ref="F47:H47"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="F48:H48"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="C64:H64"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="F67:H67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
20191127 - Quick Phase/Debug Fix
</commit_message>
<xml_diff>
--- a/res/references/First Platformer Checklist.xlsx
+++ b/res/references/First Platformer Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apauley\git\platforming101\res\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91B91CD-87E5-4339-8C4C-D12A914474A0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1EE260-BA5B-46EF-8F08-49926824A66C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="780" windowWidth="26760" windowHeight="11790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -1374,19 +1374,19 @@
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1796,8 +1796,8 @@
   </sheetPr>
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2191,7 +2191,7 @@
     <row r="28" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="149"/>
+      <c r="C28" s="124"/>
       <c r="D28" s="130">
         <f>D27+1</f>
         <v>18</v>
@@ -2207,9 +2207,9 @@
     <row r="29" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="7"/>
+      <c r="C29" s="124"/>
       <c r="D29" s="133">
-        <f t="shared" ref="D29:D36" si="3">D28+1</f>
+        <f>D28+1</f>
         <v>19</v>
       </c>
       <c r="E29" s="134" t="s">
@@ -2223,16 +2223,16 @@
     <row r="30" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="7"/>
+      <c r="C30" s="124"/>
       <c r="D30" s="130">
-        <f t="shared" si="3"/>
+        <f>D29+1</f>
         <v>20</v>
       </c>
       <c r="E30" s="131" t="s">
         <v>35</v>
       </c>
       <c r="F30" s="132" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="151" t="s">
@@ -2242,16 +2242,16 @@
     <row r="31" spans="1:8" ht="16.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="7"/>
+      <c r="C31" s="149"/>
       <c r="D31" s="133">
-        <f t="shared" si="3"/>
+        <f>D30+1</f>
         <v>21</v>
       </c>
       <c r="E31" s="134" t="s">
         <v>35</v>
       </c>
       <c r="F31" s="135" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="151" t="s">
@@ -2263,8 +2263,8 @@
       <c r="B32" s="4"/>
       <c r="C32" s="7"/>
       <c r="D32" s="130">
-        <f t="shared" si="3"/>
-        <v>22</v>
+        <f>D30+1</f>
+        <v>21</v>
       </c>
       <c r="E32" s="131" t="s">
         <v>35</v>
@@ -2282,8 +2282,8 @@
       <c r="B33" s="4"/>
       <c r="C33" s="7"/>
       <c r="D33" s="133">
-        <f t="shared" si="3"/>
-        <v>23</v>
+        <f t="shared" ref="D29:D36" si="3">D32+1</f>
+        <v>22</v>
       </c>
       <c r="E33" s="134" t="s">
         <v>35</v>
@@ -2299,7 +2299,7 @@
       <c r="C34" s="7"/>
       <c r="D34" s="130">
         <f t="shared" si="3"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E34" s="131" t="s">
         <v>35</v>
@@ -2315,7 +2315,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="133">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E35" s="134" t="s">
         <v>35</v>
@@ -2331,7 +2331,7 @@
       <c r="C36" s="7"/>
       <c r="D36" s="130">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E36" s="131" t="s">
         <v>35</v>
@@ -2367,7 +2367,7 @@
       <c r="C39" s="7"/>
       <c r="D39" s="130">
         <f>D36+1</f>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E39" s="131" t="s">
         <v>35</v>
@@ -2383,7 +2383,7 @@
       <c r="C40" s="7"/>
       <c r="D40" s="133">
         <f t="shared" ref="D40:D47" si="4">D39+1</f>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E40" s="134" t="s">
         <v>35</v>
@@ -2399,7 +2399,7 @@
       <c r="C41" s="7"/>
       <c r="D41" s="130">
         <f t="shared" si="4"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E41" s="131" t="s">
         <v>35</v>
@@ -2415,7 +2415,7 @@
       <c r="C42" s="7"/>
       <c r="D42" s="133">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E42" s="134" t="s">
         <v>35</v>
@@ -2431,7 +2431,7 @@
       <c r="C43" s="7"/>
       <c r="D43" s="130">
         <f t="shared" si="4"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E43" s="131" t="s">
         <v>35</v>
@@ -2447,7 +2447,7 @@
       <c r="C44" s="7"/>
       <c r="D44" s="133">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E44" s="134" t="s">
         <v>35</v>
@@ -2466,7 +2466,7 @@
       <c r="C45" s="7"/>
       <c r="D45" s="130">
         <f t="shared" si="4"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E45" s="131" t="s">
         <v>35</v>
@@ -2485,7 +2485,7 @@
       <c r="C46" s="7"/>
       <c r="D46" s="133">
         <f t="shared" si="4"/>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E46" s="134" t="s">
         <v>35</v>
@@ -2504,7 +2504,7 @@
       <c r="C47" s="7"/>
       <c r="D47" s="130">
         <f t="shared" si="4"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E47" s="131" t="s">
         <v>35</v>
@@ -2562,9 +2562,6 @@
     <hyperlink ref="D21:F21" location="Cd" display="d" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="D22:F22" location="Ce" display="e" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="D23:F23" location="Cf" display="f" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="D29:F29" location="Db" display="b" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="D30:F30" location="Dc" display="c" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D31:F31" location="Dd" display="d" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
     <hyperlink ref="D32:F32" location="De" display="e" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
     <hyperlink ref="D33:F33" location="Df" display="f" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
     <hyperlink ref="D34:F34" location="Dg" display="g" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
@@ -5073,11 +5070,11 @@
         <v>19</v>
       </c>
       <c r="C42" t="str">
-        <f>Checklist!E30</f>
+        <f>Checklist!E31</f>
         <v>-</v>
       </c>
       <c r="D42" t="str">
-        <f>Checklist!F30</f>
+        <f>Checklist!F31</f>
         <v>Score tracked (kills, time elapsed, etc.)</v>
       </c>
     </row>
@@ -5195,11 +5192,11 @@
         <v>20</v>
       </c>
       <c r="C52" t="str">
-        <f>Checklist!E31</f>
+        <f>Checklist!E30</f>
         <v>-</v>
       </c>
       <c r="D52" t="str">
-        <f>Checklist!F31</f>
+        <f>Checklist!F30</f>
         <v>Pause button (stop time)</v>
       </c>
     </row>
@@ -6734,77 +6731,77 @@
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="31"/>
       <c r="C44" s="75"/>
-      <c r="D44" s="164" t="s">
+      <c r="D44" s="160" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="164"/>
-      <c r="F44" s="164"/>
-      <c r="G44" s="164"/>
+      <c r="E44" s="160"/>
+      <c r="F44" s="160"/>
+      <c r="G44" s="160"/>
       <c r="H44" s="75"/>
       <c r="I44" s="33"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="31"/>
-      <c r="C45" s="162" t="s">
+      <c r="C45" s="161" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="162"/>
+      <c r="D45" s="161"/>
       <c r="E45" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="F45" s="162">
+      <c r="F45" s="161">
         <v>9001</v>
       </c>
-      <c r="G45" s="162"/>
-      <c r="H45" s="162"/>
+      <c r="G45" s="161"/>
+      <c r="H45" s="161"/>
       <c r="I45" s="33"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" s="31"/>
-      <c r="C46" s="160" t="s">
+      <c r="C46" s="162" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="160"/>
+      <c r="D46" s="162"/>
       <c r="E46" s="120" t="s">
         <v>54</v>
       </c>
-      <c r="F46" s="160">
+      <c r="F46" s="162">
         <v>8999</v>
       </c>
-      <c r="G46" s="160"/>
-      <c r="H46" s="160"/>
+      <c r="G46" s="162"/>
+      <c r="H46" s="162"/>
       <c r="I46" s="33"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="31"/>
-      <c r="C47" s="160" t="s">
+      <c r="C47" s="162" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="160"/>
+      <c r="D47" s="162"/>
       <c r="E47" s="120" t="s">
         <v>54</v>
       </c>
-      <c r="F47" s="160">
+      <c r="F47" s="162">
         <v>1337</v>
       </c>
-      <c r="G47" s="160"/>
-      <c r="H47" s="160"/>
+      <c r="G47" s="162"/>
+      <c r="H47" s="162"/>
       <c r="I47" s="33"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="31"/>
-      <c r="C48" s="160" t="s">
+      <c r="C48" s="162" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="160"/>
+      <c r="D48" s="162"/>
       <c r="E48" s="120" t="s">
         <v>54</v>
       </c>
-      <c r="F48" s="160">
+      <c r="F48" s="162">
         <v>-5</v>
       </c>
-      <c r="G48" s="160"/>
-      <c r="H48" s="160"/>
+      <c r="G48" s="162"/>
+      <c r="H48" s="162"/>
       <c r="I48" s="33"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
@@ -7025,50 +7022,50 @@
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="31"/>
-      <c r="C66" s="160" t="s">
+      <c r="C66" s="162" t="s">
         <v>65</v>
       </c>
-      <c r="D66" s="160"/>
+      <c r="D66" s="162"/>
       <c r="E66" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="F66" s="161" t="s">
+      <c r="F66" s="163" t="s">
         <v>66</v>
       </c>
-      <c r="G66" s="161"/>
-      <c r="H66" s="161"/>
+      <c r="G66" s="163"/>
+      <c r="H66" s="163"/>
       <c r="I66" s="33"/>
     </row>
     <row r="67" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="31"/>
-      <c r="C67" s="162" t="s">
+      <c r="C67" s="161" t="s">
         <v>68</v>
       </c>
-      <c r="D67" s="162"/>
+      <c r="D67" s="161"/>
       <c r="E67" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="F67" s="163" t="s">
+      <c r="F67" s="164" t="s">
         <v>66</v>
       </c>
-      <c r="G67" s="163"/>
-      <c r="H67" s="163"/>
+      <c r="G67" s="164"/>
+      <c r="H67" s="164"/>
       <c r="I67" s="33"/>
     </row>
     <row r="68" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="31"/>
-      <c r="C68" s="160" t="s">
+      <c r="C68" s="162" t="s">
         <v>67</v>
       </c>
-      <c r="D68" s="160"/>
+      <c r="D68" s="162"/>
       <c r="E68" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="F68" s="161" t="s">
+      <c r="F68" s="163" t="s">
         <v>66</v>
       </c>
-      <c r="G68" s="161"/>
-      <c r="H68" s="161"/>
+      <c r="G68" s="163"/>
+      <c r="H68" s="163"/>
       <c r="I68" s="33"/>
     </row>
     <row r="69" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7905,6 +7902,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="C64:H64"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="F67:H67"/>
     <mergeCell ref="D44:G44"/>
     <mergeCell ref="D57:G57"/>
     <mergeCell ref="D58:G58"/>
@@ -7918,13 +7922,6 @@
     <mergeCell ref="F47:H47"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="F48:H48"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="C64:H64"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="F67:H67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>